<commit_message>
Fix pricing spreadsheet col E Tiers error
</commit_message>
<xml_diff>
--- a/_assets/documents/cloud-gov-cost-estimator.xlsx
+++ b/_assets/documents/cloud-gov-cost-estimator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterdburkholder/Projects/cloud-gov/cg-site/_assets/documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterdburkholder/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F2CCC5-A8FF-6241-AE0E-4F14A78F5FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A470298C-01F6-D747-A90E-711FF4271ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3360" yWindow="500" windowWidth="47840" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="191">
   <si>
     <t>Estimated Price</t>
   </si>
@@ -644,6 +644,9 @@
   </si>
   <si>
     <t>Initial version</t>
+  </si>
+  <si>
+    <t>Fix col E of Tiers</t>
   </si>
 </sst>
 </file>
@@ -657,7 +660,7 @@
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.0000"/>
     <numFmt numFmtId="167" formatCode="0\ &quot;Gb&quot;"/>
     <numFmt numFmtId="168" formatCode="0\ &quot;Hrs&quot;"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -723,6 +726,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1441,7 +1445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1708,10 +1712,6 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1723,16 +1723,18 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="69">
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1818,12 +1820,7 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="169" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1831,6 +1828,14 @@
           <color rgb="FF4A535C"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3232,10 +3237,10 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}" name="Table12" displayName="Table12" ref="A39:C49" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}" name="Table12" displayName="Table12" ref="A39:C49" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8">
   <autoFilter ref="A39:C49" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6F594386-932F-3745-B570-1D36152A4BED}" name="Version" dataDxfId="0" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{6F594386-932F-3745-B570-1D36152A4BED}" name="Version" dataDxfId="7" dataCellStyle="Comma"/>
     <tableColumn id="2" xr3:uid="{98BA1600-A7B8-2742-AF88-1C465CCF83D5}" name="Date"/>
     <tableColumn id="3" xr3:uid="{A3A06425-E98A-E042-A27B-C92165F08BCF}" name="Notes"/>
   </tableColumns>
@@ -3448,7 +3453,7 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3478,14 +3483,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="98.25" customHeight="1" x14ac:dyDescent="1.05">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="106" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4894,13 +4899,13 @@
       </c>
     </row>
     <row r="39" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="104" t="s">
+      <c r="A39" s="102" t="s">
         <v>183</v>
       </c>
-      <c r="B39" s="105" t="s">
+      <c r="B39" s="103" t="s">
         <v>184</v>
       </c>
-      <c r="C39" s="106" t="s">
+      <c r="C39" s="104" t="s">
         <v>185</v>
       </c>
       <c r="E39" s="24" t="str">
@@ -4930,13 +4935,13 @@
       </c>
     </row>
     <row r="40" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="107">
+      <c r="A40" s="105">
         <v>1</v>
       </c>
-      <c r="B40" s="103">
+      <c r="B40" s="101">
         <v>45748</v>
       </c>
-      <c r="C40" s="102" t="s">
+      <c r="C40" s="100" t="s">
         <v>189</v>
       </c>
       <c r="E40" s="18" t="str">
@@ -4984,13 +4989,13 @@
       </c>
     </row>
     <row r="41" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="107">
+      <c r="A41" s="105">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B41" s="103">
+      <c r="B41" s="101">
         <v>45749</v>
       </c>
-      <c r="C41" s="102" t="s">
+      <c r="C41" s="100" t="s">
         <v>186</v>
       </c>
       <c r="E41" s="24" t="str">
@@ -5040,8 +5045,8 @@
       </c>
     </row>
     <row r="42" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="107"/>
-      <c r="C42" s="102" t="s">
+      <c r="A42" s="105"/>
+      <c r="C42" s="100" t="s">
         <v>187</v>
       </c>
       <c r="E42" s="18" t="str">
@@ -5091,8 +5096,8 @@
       </c>
     </row>
     <row r="43" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="107"/>
-      <c r="C43" s="102" t="s">
+      <c r="A43" s="105"/>
+      <c r="C43" s="100" t="s">
         <v>188</v>
       </c>
       <c r="E43" s="54" t="str">
@@ -5120,31 +5125,39 @@
       <c r="Q43" s="98"/>
     </row>
     <row r="44" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="107"/>
+      <c r="A44" s="105">
+        <v>1.2</v>
+      </c>
+      <c r="B44" s="101">
+        <v>45756</v>
+      </c>
+      <c r="C44" s="108" t="s">
+        <v>190</v>
+      </c>
       <c r="J44" s="4"/>
     </row>
     <row r="45" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="107"/>
+      <c r="A45" s="105"/>
       <c r="J45" s="4"/>
     </row>
     <row r="46" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="107"/>
+      <c r="A46" s="105"/>
       <c r="J46" s="4"/>
     </row>
     <row r="47" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="107"/>
+      <c r="A47" s="105"/>
       <c r="J47" s="4"/>
     </row>
     <row r="48" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="107"/>
+      <c r="A48" s="105"/>
       <c r="J48" s="4"/>
     </row>
     <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="107"/>
+      <c r="A49" s="105"/>
       <c r="J49" s="4"/>
     </row>
     <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="107"/>
+      <c r="A50" s="105"/>
       <c r="J50" s="4"/>
     </row>
     <row r="51" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6158,37 +6171,37 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="B10 J14:J43 B15">
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R15">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R19:R29">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R33:R37">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R41:R42">
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6216,7 +6229,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
All zeros on main sheet; mv example to end sheet
</commit_message>
<xml_diff>
--- a/_assets/documents/cloud-gov-cost-estimator.xlsx
+++ b/_assets/documents/cloud-gov-cost-estimator.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterdburkholder/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterdburkholder/Projects/cloud-gov/site/_assets/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C76884D-41E9-5148-8AD7-AB77D07A070A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5274FA16-971E-7A40-85CA-ED6AD0EAA238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="500" windowWidth="47840" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="500" windowWidth="47840" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
     <sheet name="Cloud.gov Tiers" sheetId="2" r:id="rId2"/>
     <sheet name="AWS Service Prices" sheetId="3" r:id="rId3"/>
+    <sheet name="Example worksheet" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="AWS_RDS_Instances" localSheetId="3">'Example worksheet'!$E$13:$K$43</definedName>
     <definedName name="AWS_RDS_Instances">Worksheet!$E$13:$K$43</definedName>
     <definedName name="AwsElasticCachePrices">'AWS Service Prices'!$A$44:$E$48</definedName>
     <definedName name="AwsOpensearchPrices">'AWS Service Prices'!$A$33:$E$43</definedName>
@@ -68,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="195">
   <si>
     <t>Estimated Price</t>
   </si>
@@ -650,6 +652,19 @@
   </si>
   <si>
     <t>Conditional formating</t>
+  </si>
+  <si>
+    <t>Instructions:
+- Update numbers in yellow, with red borders, to generate your own estimate.
+- For services that AWS bills hourly, we bill based on the total instances operating at the end of the month. 
+- To create an estimate, average your usage over the month.
+- See "Example Worksheet" for minimal-cost example system</t>
+  </si>
+  <si>
+    <t>Zeros on main sheet</t>
+  </si>
+  <si>
+    <t>Mv example to end</t>
   </si>
 </sst>
 </file>
@@ -1448,7 +1463,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1728,6 +1743,7 @@
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1737,7 +1753,1097 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="76">
+  <dxfs count="122">
+    <dxf>
+      <numFmt numFmtId="169" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF4A535C"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF284E3F"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="0\ &quot;Gb&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFFF0000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFFF0000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFFF0000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFFF0000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF284E3F"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0\ &quot;Hrs&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF284E3F"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="0\ &quot;Gb&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFFF0000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFFF0000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFFF0000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFFF0000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF284E3F"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+        <family val="2"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="0\ &quot;Gb&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFFF0000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFFF0000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFFF0000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFFF0000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.0000"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF284E3F"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="0\ &quot;Gb&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFFF0000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFFF0000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFFF0000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFFF0000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -3071,54 +4177,54 @@
   </dxfs>
   <tableStyles count="10">
     <tableStyle name="Worksheet-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="75"/>
-      <tableStyleElement type="firstRowStripe" dxfId="74"/>
-      <tableStyleElement type="secondRowStripe" dxfId="73"/>
+      <tableStyleElement type="headerRow" dxfId="121"/>
+      <tableStyleElement type="firstRowStripe" dxfId="120"/>
+      <tableStyleElement type="secondRowStripe" dxfId="119"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="72"/>
-      <tableStyleElement type="firstRowStripe" dxfId="71"/>
-      <tableStyleElement type="secondRowStripe" dxfId="70"/>
+      <tableStyleElement type="headerRow" dxfId="118"/>
+      <tableStyleElement type="firstRowStripe" dxfId="117"/>
+      <tableStyleElement type="secondRowStripe" dxfId="116"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="headerRow" dxfId="69"/>
-      <tableStyleElement type="firstRowStripe" dxfId="68"/>
-      <tableStyleElement type="secondRowStripe" dxfId="67"/>
+      <tableStyleElement type="headerRow" dxfId="115"/>
+      <tableStyleElement type="firstRowStripe" dxfId="114"/>
+      <tableStyleElement type="secondRowStripe" dxfId="113"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 4" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
-      <tableStyleElement type="headerRow" dxfId="66"/>
-      <tableStyleElement type="firstRowStripe" dxfId="65"/>
-      <tableStyleElement type="secondRowStripe" dxfId="64"/>
+      <tableStyleElement type="headerRow" dxfId="112"/>
+      <tableStyleElement type="firstRowStripe" dxfId="111"/>
+      <tableStyleElement type="secondRowStripe" dxfId="110"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 5" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
-      <tableStyleElement type="headerRow" dxfId="63"/>
-      <tableStyleElement type="firstRowStripe" dxfId="62"/>
-      <tableStyleElement type="secondRowStripe" dxfId="61"/>
+      <tableStyleElement type="headerRow" dxfId="109"/>
+      <tableStyleElement type="firstRowStripe" dxfId="108"/>
+      <tableStyleElement type="secondRowStripe" dxfId="107"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 6" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
-      <tableStyleElement type="headerRow" dxfId="60"/>
-      <tableStyleElement type="firstRowStripe" dxfId="59"/>
-      <tableStyleElement type="secondRowStripe" dxfId="58"/>
+      <tableStyleElement type="headerRow" dxfId="106"/>
+      <tableStyleElement type="firstRowStripe" dxfId="105"/>
+      <tableStyleElement type="secondRowStripe" dxfId="104"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 7" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF06000000}">
-      <tableStyleElement type="headerRow" dxfId="57"/>
-      <tableStyleElement type="firstRowStripe" dxfId="56"/>
-      <tableStyleElement type="secondRowStripe" dxfId="55"/>
+      <tableStyleElement type="headerRow" dxfId="103"/>
+      <tableStyleElement type="firstRowStripe" dxfId="102"/>
+      <tableStyleElement type="secondRowStripe" dxfId="101"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 8" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF07000000}">
-      <tableStyleElement type="headerRow" dxfId="54"/>
-      <tableStyleElement type="firstRowStripe" dxfId="53"/>
-      <tableStyleElement type="secondRowStripe" dxfId="52"/>
+      <tableStyleElement type="headerRow" dxfId="100"/>
+      <tableStyleElement type="firstRowStripe" dxfId="99"/>
+      <tableStyleElement type="secondRowStripe" dxfId="98"/>
     </tableStyle>
     <tableStyle name="Cloud.gov Tiers-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF08000000}">
-      <tableStyleElement type="headerRow" dxfId="51"/>
-      <tableStyleElement type="firstRowStripe" dxfId="50"/>
-      <tableStyleElement type="secondRowStripe" dxfId="49"/>
+      <tableStyleElement type="headerRow" dxfId="97"/>
+      <tableStyleElement type="firstRowStripe" dxfId="96"/>
+      <tableStyleElement type="secondRowStripe" dxfId="95"/>
     </tableStyle>
     <tableStyle name="Cloud.gov Tiers-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF09000000}">
-      <tableStyleElement type="headerRow" dxfId="48"/>
-      <tableStyleElement type="firstRowStripe" dxfId="47"/>
-      <tableStyleElement type="secondRowStripe" dxfId="46"/>
+      <tableStyleElement type="headerRow" dxfId="94"/>
+      <tableStyleElement type="firstRowStripe" dxfId="93"/>
+      <tableStyleElement type="secondRowStripe" dxfId="92"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -3135,20 +4241,20 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A4:F5">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Credits" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tier Name" dataDxfId="44">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Credits" dataDxfId="91"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tier Name" dataDxfId="90">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.Tier, VLOOKUP(MIN(IF('Cloud.gov Tiers'!$B$11:$B$28&gt;=A5, 'Cloud.gov Tiers'!$B$11:$B$28)), 'Cloud.gov Tiers'!$B$11:$E$28, 4, FALSE), VLOOKUP(_xlpm.Tier, 'Cloud.gov Tiers'!$E$10:$F$28, 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Credits Remaining_x000a_in Tier" dataDxfId="43">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Credits Remaining_x000a_in Tier" dataDxfId="89">
       <calculatedColumnFormula>VLOOKUP(Table_1[[#This Row],[Tier Name]], 'Cloud.gov Tiers'!A11:B27, 2,FALSE)-Table_1[[#This Row],[Credits]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Yearly_x000a_Platform Total" dataDxfId="42">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Yearly_x000a_Platform Total" dataDxfId="88">
       <calculatedColumnFormula>IF(B5="Custom", ROUNDUP(A5/1000,0)*'Cloud.gov Tiers'!$H$28, VLOOKUP(B5, 'Cloud.gov Tiers'!$F$11:$H$27, 3, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Support Total" dataDxfId="41">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Support Total" dataDxfId="87">
       <calculatedColumnFormula>C15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name=" YearlyTotal Cost" dataDxfId="40">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name=" YearlyTotal Cost" dataDxfId="86">
       <calculatedColumnFormula>D5+E5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3182,27 +4288,175 @@
 </table>
 </file>
 
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{4C37D040-F691-2C49-BE22-816489BFD4D2}" name="Table_112" displayName="Table_112" ref="A4:F5">
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{657244D4-FE4C-D44C-B48B-43E7FA139C6B}" name="Credits" dataDxfId="31">
+      <calculatedColumnFormula>C10+SUM(B19:B23)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{B168D809-F848-8A4F-B241-57C6EF027C29}" name="Tier Name" dataDxfId="30">
+      <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.Tier, VLOOKUP(MIN(IF('Cloud.gov Tiers'!$B$11:$B$28&gt;=A5, 'Cloud.gov Tiers'!$B$11:$B$28)), 'Cloud.gov Tiers'!$B$11:$E$28, 4, FALSE), VLOOKUP(_xlpm.Tier, 'Cloud.gov Tiers'!$E$10:$F$28, 2, FALSE))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{172BAC85-F7D2-7D4C-9C26-72C7C85DB56F}" name="Credits Remaining_x000a_in Tier" dataDxfId="29">
+      <calculatedColumnFormula>VLOOKUP(Table_112[[#This Row],[Tier Name]], 'Cloud.gov Tiers'!A11:B27, 2,FALSE)-Table_112[[#This Row],[Credits]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{19498A2C-21A7-B740-9DD5-D095ED0DD812}" name="Yearly_x000a_Platform Total" dataDxfId="28">
+      <calculatedColumnFormula>IF(B5="Custom", ROUNDUP(A5/1000,0)*'Cloud.gov Tiers'!$H$28, VLOOKUP(B5, 'Cloud.gov Tiers'!$F$11:$H$27, 3, FALSE))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{A475BA76-45A9-EF46-8FAE-2B381389CF6E}" name="Support Total" dataDxfId="27">
+      <calculatedColumnFormula>C15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{CFD58EB9-7FC4-3640-859D-34D006952E97}" name=" YearlyTotal Cost" dataDxfId="26">
+      <calculatedColumnFormula>D5+E5</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="Worksheet-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{432B26DD-C481-9945-89E7-FEF42FEDB769}" name="Table_214" displayName="Table_214" ref="A9:C10">
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8D2D857E-9AA6-5D4F-A4AF-373B7168526E}" name="Resource"/>
+    <tableColumn id="2" xr3:uid="{4FAE5D4B-8591-7D41-A69E-501EE57C6C41}" name="Quantity" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{FD66B2C4-D49F-1C43-9A30-DE1F21B9FD5B}" name="Credits">
+      <calculatedColumnFormula>B10*'Cloud.gov Tiers'!B3</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="Worksheet-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{3AE58A18-ABB7-FC4E-9D28-06F1CAA78773}" name="Table_315" displayName="Table_315" ref="E9:K10">
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{8901DDBE-58BA-8F4F-9D7C-2A2800A70157}" name="Offering" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{3C07AF3B-6C04-4348-A1E4-AEF634AB5F2C}" name="Description" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{50B2B6E3-7A84-CC41-A61F-9E7C70E4AC01}" name="Units" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{99748816-FA07-B948-9F02-BAFA13C63BF0}" name="Dimension" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{B4686AED-FFA8-0F4F-8CF1-A28CBB869F59}" name="GB per credit" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{C47C64B0-2C30-0043-A34C-7F0E810B25DC}" name="Quantity (GB)" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{D0A5DC61-9EB0-294B-94B0-91D19A5D6E7E}" name="Credits" dataDxfId="18">
+      <calculatedColumnFormula>ROUNDUP(Table_315[[#This Row],[Quantity (GB)]]/Table_315[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="Worksheet-style 3" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{4E799C99-FC6F-6740-8C47-548247059706}" name="Table_416" displayName="Table_416" ref="M9:S10">
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{CC812881-5649-1A4C-8C45-49D7808E0D1A}" name="Offering"/>
+    <tableColumn id="2" xr3:uid="{46204D59-C3E2-174B-9C58-1DB2BB6988C8}" name="Description"/>
+    <tableColumn id="4" xr3:uid="{C3D129A0-D876-D446-9BED-4CE757DA989E}" name="Units"/>
+    <tableColumn id="5" xr3:uid="{8159B7E1-3CBB-384F-9C82-294839F55CB1}" name="Dimension" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{6374D1D7-2C6C-674A-9B2C-B5EA274BAEAC}" name="GB per credit" dataDxfId="16">
+      <calculatedColumnFormula>'AWS Service Prices'!K5*'AWS Service Prices'!M5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{84537EB8-58A4-A645-9A18-A322EFB5D6C3}" name="Quantity (GB)" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{06CE2B03-0479-2148-9683-4F1675E4317C}" name="Credits" dataDxfId="14">
+      <calculatedColumnFormula>ROUNDUP(Table_416[[#This Row],[Quantity (GB)]]/Table_416[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="Worksheet-style 4" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{DD38669A-9AE2-BA49-AF4A-F9D5CEFDB233}" name="Table_517" displayName="Table_517" ref="A14:C15">
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{E0798FE9-1580-1B43-B088-25897B8976F6}" name="Rate/Hour"/>
+    <tableColumn id="2" xr3:uid="{4F69F05E-31AF-C644-B087-9847D08BB3A0}" name="Hours" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{35F99F2C-96B5-1244-8BF2-D8FA71D1A5B2}" name="Total">
+      <calculatedColumnFormula>A15*B15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="Worksheet-style 5" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{53A578BF-BA5A-7843-972B-EBD4EA7AD1DD}" name="Table_618" displayName="Table_618" ref="M14:S15" dataDxfId="12">
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{3024083C-5ED0-8D4D-8D1A-D4BD5916AE47}" name="Offering" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{3D92B04D-745E-2A49-991D-C00C27907719}" name="Description" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{50C39022-EBD5-9B42-84DD-C507ED702117}" name="Units" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{9759566D-ABA1-0943-92F2-2B5501002EE3}" name="Dimension" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{4A17BDB6-3CD8-BF43-B5F9-82D2A2C35A0C}" name="GB per credit" dataDxfId="7">
+      <calculatedColumnFormula>'AWS Service Prices'!K4*'AWS Service Prices'!M4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{056FCEF1-5646-814F-8034-1E8AC53C910D}" name="Quantity (GB)" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{DAEA814F-05EA-764E-8533-FE0EF6F3B132}" name="Credits" dataDxfId="5">
+      <calculatedColumnFormula>ROUNDUP(Table_618[[#This Row],[Quantity (GB)]]/Table_618[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="Worksheet-style 6" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{FE828B4F-17FC-1B43-9333-8BB094B53DDC}" name="Table_719" displayName="Table_719" ref="A18:B23">
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{91890D40-9E6C-D740-B06A-0795C2CC0DC6}" name="Service"/>
+    <tableColumn id="2" xr3:uid="{6BAAE4FE-CE19-094E-871D-D2B9802CB9CB}" name="Credits"/>
+  </tableColumns>
+  <tableStyleInfo name="Worksheet-style 7" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{147CA396-DF94-254C-96FD-3C5EBD9F03F2}" name="Table_820" displayName="Table_820" ref="M40:S42">
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{AECC13D3-8D85-144F-B6DB-5501458D6B29}" name="Offering"/>
+    <tableColumn id="2" xr3:uid="{B074D0B3-B914-AB4F-8066-81B90B3261D8}" name="Description"/>
+    <tableColumn id="4" xr3:uid="{202C8C30-FD4E-6D40-9EBF-642B8C7AE181}" name="Units"/>
+    <tableColumn id="5" xr3:uid="{CA6A3A17-2747-AF44-8119-FC05700B8D5C}" name="Dimension"/>
+    <tableColumn id="3" xr3:uid="{C6C6ED4B-9612-3F48-9D18-472E70646A28}" name="Units/Credit" dataDxfId="4">
+      <calculatedColumnFormula>'AWS Service Prices'!K6*'AWS Service Prices'!M6</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{76CCCB3A-2B18-4C42-9DB6-C570AFD6FB75}" name="Quantity"/>
+    <tableColumn id="7" xr3:uid="{A024F374-2C63-444D-95DA-745B84ABCFE7}" name="Credits" dataDxfId="3">
+      <calculatedColumnFormula>ROUNDUP(Table_820[[#This Row],[Quantity]]/Table_820[[#This Row],[Units/Credit]],0)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="Worksheet-style 8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A9:C10">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Resource"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Quantity" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Quantity" dataDxfId="85"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Credits"/>
   </tableColumns>
   <tableStyleInfo name="Worksheet-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{333F2C22-64BE-8A4A-A52E-89FC6130AD21}" name="Table1221" displayName="Table1221" ref="A39:C49" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1">
+  <autoFilter ref="A39:C49" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{0A95F7D5-D48D-864F-84FF-73515D627597}" name="Version" dataDxfId="0" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{1427474E-5614-2046-B78C-0448E419A1D9}" name="Date"/>
+    <tableColumn id="3" xr3:uid="{CAF26780-3593-1540-85AB-2E9EB898659F}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="Cloud.gov Tiers-style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_3" displayName="Table_3" ref="E9:K10">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Offering" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Description" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Dimension" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="GB per credit" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Quantity (GB)" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Credits" dataDxfId="32">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Offering" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Description" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Dimension" dataDxfId="81"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="GB per credit" dataDxfId="80"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Quantity (GB)" dataDxfId="79"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Credits" dataDxfId="78">
       <calculatedColumnFormula>ROUNDUP(Table_3[[#This Row],[Quantity (GB)]]/Table_3[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3216,12 +4470,12 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Offering"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Units"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Dimension" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{CDA60C5E-AE6A-324F-8F61-A71F1A0A8966}" name="GB per credit" dataDxfId="30">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Dimension" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{CDA60C5E-AE6A-324F-8F61-A71F1A0A8966}" name="GB per credit" dataDxfId="76">
       <calculatedColumnFormula>'AWS Service Prices'!K5*'AWS Service Prices'!M5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Quantity (GB)" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Credits" dataDxfId="28">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Quantity (GB)" dataDxfId="75"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Credits" dataDxfId="74">
       <calculatedColumnFormula>ROUNDUP(Table_4[[#This Row],[Quantity (GB)]]/Table_4[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3233,7 +4487,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_5" displayName="Table_5" ref="A14:C15">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Rate/Hour"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Hours" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Hours" dataDxfId="73"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Total"/>
   </tableColumns>
   <tableStyleInfo name="Worksheet-style 5" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
@@ -3241,17 +4495,17 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_6" displayName="Table_6" ref="M14:S15" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_6" displayName="Table_6" ref="M14:S15" dataDxfId="72">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Offering" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Description" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Units" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Dimension" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{807927EE-801B-8148-9BA1-5FE9186170F2}" name="GB per credit" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Offering" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Description" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Units" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Dimension" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{807927EE-801B-8148-9BA1-5FE9186170F2}" name="GB per credit" dataDxfId="67">
       <calculatedColumnFormula>'AWS Service Prices'!K4*'AWS Service Prices'!M4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Quantity (GB)" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Credits" dataDxfId="19">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Quantity (GB)" dataDxfId="66"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Credits" dataDxfId="65">
       <calculatedColumnFormula>ROUNDUP(Table_6[[#This Row],[Quantity (GB)]]/Table_6[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3276,11 +4530,11 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Units"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Dimension"/>
-    <tableColumn id="3" xr3:uid="{A30E673E-5221-9442-BA33-5D5CC8E273B5}" name="Units/Credit" dataDxfId="18">
+    <tableColumn id="3" xr3:uid="{A30E673E-5221-9442-BA33-5D5CC8E273B5}" name="Units/Credit" dataDxfId="64">
       <calculatedColumnFormula>'AWS Service Prices'!K6*'AWS Service Prices'!M6</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Quantity"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Credits" dataDxfId="17">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Credits" dataDxfId="63">
       <calculatedColumnFormula>ROUNDUP(Table_8[[#This Row],[Quantity]]/Table_8[[#This Row],[Units/Credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3289,10 +4543,10 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}" name="Table12" displayName="Table12" ref="A39:C49" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}" name="Table12" displayName="Table12" ref="A39:C49" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61">
   <autoFilter ref="A39:C49" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6F594386-932F-3745-B570-1D36152A4BED}" name="Version" dataDxfId="14" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{6F594386-932F-3745-B570-1D36152A4BED}" name="Version" dataDxfId="60" dataCellStyle="Comma"/>
     <tableColumn id="2" xr3:uid="{98BA1600-A7B8-2742-AF88-1C465CCF83D5}" name="Date"/>
     <tableColumn id="3" xr3:uid="{A3A06425-E98A-E042-A27B-C92165F08BCF}" name="Notes"/>
   </tableColumns>
@@ -3504,8 +4758,8 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3535,14 +4789,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="98.25" customHeight="1" x14ac:dyDescent="1.05">
-      <c r="A1" s="107" t="s">
-        <v>182</v>
-      </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
+      <c r="A1" s="108" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3579,7 +4833,7 @@
     <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="81">
         <f>C10+SUM(B19:B23)</f>
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="B5" s="82" t="str" cm="1">
         <f t="array" ref="B5">_xlfn.LET(_xlpm.Tier, VLOOKUP(MIN(IF('Cloud.gov Tiers'!$B$11:$B$28&gt;=A5, 'Cloud.gov Tiers'!$B$11:$B$28)), 'Cloud.gov Tiers'!$B$11:$E$28, 4, FALSE), VLOOKUP(_xlpm.Tier, 'Cloud.gov Tiers'!$E$10:$F$28, 2, FALSE))</f>
@@ -3587,7 +4841,7 @@
       </c>
       <c r="C5" s="76">
         <f>VLOOKUP(Table_1[[#This Row],[Tier Name]], 'Cloud.gov Tiers'!A11:B27, 2,FALSE)-Table_1[[#This Row],[Credits]]</f>
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="D5" s="77">
         <f>IF(B5="Custom", ROUNDUP(A5/1000,0)*'Cloud.gov Tiers'!$H$28, VLOOKUP(B5, 'Cloud.gov Tiers'!$F$11:$H$27, 3, FALSE))</f>
@@ -3595,11 +4849,11 @@
       </c>
       <c r="E5" s="77">
         <f>C15</f>
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="F5" s="84">
         <f>D5+E5</f>
-        <v>32500</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3676,11 +4930,11 @@
         <v>15</v>
       </c>
       <c r="B10" s="85">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C10" s="12">
         <f>B10*'Cloud.gov Tiers'!B3</f>
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="E10" s="39" t="s">
         <v>16</v>
@@ -3698,11 +4952,11 @@
         <v>100</v>
       </c>
       <c r="J10" s="85">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="K10" s="42">
         <f>ROUNDUP(Table_3[[#This Row],[Quantity (GB)]]/Table_3[[#This Row],[GB per credit]],0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M10" s="13" t="s">
         <v>7</v>
@@ -3721,11 +4975,11 @@
         <v>400</v>
       </c>
       <c r="R10" s="85">
-        <v>401</v>
+        <v>0</v>
       </c>
       <c r="S10" s="42">
         <f>ROUNDUP(Table_4[[#This Row],[Quantity (GB)]]/Table_4[[#This Row],[GB per credit]],0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3796,11 +5050,11 @@
         <v>1</v>
       </c>
       <c r="J14" s="20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K14" s="90">
         <f>I14*J14</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M14" s="5" t="s">
         <v>10</v>
@@ -3829,11 +5083,11 @@
         <v>250</v>
       </c>
       <c r="B15" s="86">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C15" s="23">
         <f>A15*B15</f>
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="E15" s="24" t="str">
         <v>AWS RDS</v>
@@ -3925,11 +5179,11 @@
         <v>4</v>
       </c>
       <c r="J17" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" s="90">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>40</v>
@@ -3993,7 +5247,7 @@
       </c>
       <c r="B19" s="31">
         <f t="array" ref="B19">Worksheet!$S$10</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E19" s="24" t="str">
         <v>AWS RDS</v>
@@ -4047,7 +5301,7 @@
       </c>
       <c r="B20" s="34">
         <f t="array" ref="B20">SUM(K14:K43) + Worksheet!$K$10</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E20" s="18" t="str">
         <v>AWS RDS</v>
@@ -4206,7 +5460,7 @@
       </c>
       <c r="B23" s="37">
         <f>SUM(Table_8[Credits])</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E23" s="24" t="str">
         <v>AWS RDS</v>
@@ -5089,11 +6343,11 @@
         <v>150000</v>
       </c>
       <c r="R41" s="93">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S41" s="97">
         <f>ROUNDUP(Table_8[[#This Row],[Quantity]]/Table_8[[#This Row],[Units/Credit]],0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -5140,11 +6394,11 @@
         <v>120</v>
       </c>
       <c r="R42" s="94">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S42" s="96">
         <f>ROUNDUP(Table_8[[#This Row],[Quantity]]/Table_8[[#This Row],[Units/Credit]],0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -5201,11 +6455,22 @@
       <c r="J45" s="4"/>
     </row>
     <row r="46" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="105"/>
+      <c r="A46" s="105">
+        <v>1.4</v>
+      </c>
+      <c r="B46" s="101">
+        <v>45775</v>
+      </c>
+      <c r="C46" s="106" t="s">
+        <v>193</v>
+      </c>
       <c r="J46" s="4"/>
     </row>
     <row r="47" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="105"/>
+      <c r="C47" s="106" t="s">
+        <v>194</v>
+      </c>
       <c r="J47" s="4"/>
     </row>
     <row r="48" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6231,72 +7496,72 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="B10 J14:J43 B15">
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="notEqual">
+    <cfRule type="cellIs" dxfId="59" priority="17" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="12" priority="6">
+    <cfRule type="expression" dxfId="58" priority="6">
       <formula>$J$10&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:F43">
-    <cfRule type="expression" dxfId="11" priority="7">
+    <cfRule type="expression" dxfId="57" priority="7">
       <formula>$J14&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="notEqual">
+    <cfRule type="cellIs" dxfId="56" priority="8" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="55" priority="4">
       <formula>$R10&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="54" priority="5">
       <formula>$R15&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19:N29">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="53" priority="3">
       <formula>$R19&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N33:N37">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="52" priority="2">
       <formula>$R33&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N41:N42">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="51" priority="1">
       <formula>$R41&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="notEqual">
+    <cfRule type="cellIs" dxfId="50" priority="10" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R15">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="notEqual">
+    <cfRule type="cellIs" dxfId="49" priority="9" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R19:R29">
-    <cfRule type="cellIs" dxfId="2" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="48" priority="12" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R33:R37">
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="notEqual">
+    <cfRule type="cellIs" dxfId="47" priority="11" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R41:R42">
-    <cfRule type="cellIs" dxfId="0" priority="14" operator="notEqual">
+    <cfRule type="cellIs" dxfId="46" priority="14" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7978,7 +9243,7 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3:M3"/>
     </sheetView>
   </sheetViews>
@@ -10367,4 +11632,2820 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB4464BB-8819-134A-A622-87B69BA68B40}">
+  <sheetPr>
+    <tabColor rgb="FF4A86E8"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:Y1000"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" style="107" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" style="107" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="107" customWidth="1"/>
+    <col min="4" max="4" width="15" style="107" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="107" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" style="107" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="107" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="107" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="107"/>
+    <col min="10" max="10" width="14.6640625" style="107" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" style="107" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" style="107" customWidth="1"/>
+    <col min="13" max="13" width="18.83203125" style="107" customWidth="1"/>
+    <col min="14" max="14" width="36.6640625" style="107" customWidth="1"/>
+    <col min="15" max="15" width="19.5" style="107" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" style="107" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" style="107" customWidth="1"/>
+    <col min="18" max="18" width="11.83203125" style="107" customWidth="1"/>
+    <col min="19" max="19" width="9.33203125" style="107" customWidth="1"/>
+    <col min="20" max="21" width="12.6640625" style="107"/>
+    <col min="22" max="22" width="15.1640625" style="107" customWidth="1"/>
+    <col min="23" max="23" width="21.33203125" style="107" customWidth="1"/>
+    <col min="24" max="24" width="23" style="107" customWidth="1"/>
+    <col min="25" max="25" width="16.5" style="107" customWidth="1"/>
+    <col min="26" max="16384" width="12.6640625" style="107"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="98.25" customHeight="1" x14ac:dyDescent="1.05">
+      <c r="A1" s="108" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:19" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="80" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" s="80" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" s="79" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="83" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="81">
+        <f>C10+SUM(B19:B23)</f>
+        <v>48</v>
+      </c>
+      <c r="B5" s="82" t="str" cm="1">
+        <f t="array" ref="B5">_xlfn.LET(_xlpm.Tier, VLOOKUP(MIN(IF('Cloud.gov Tiers'!$B$11:$B$28&gt;=A5, 'Cloud.gov Tiers'!$B$11:$B$28)), 'Cloud.gov Tiers'!$B$11:$E$28, 4, FALSE), VLOOKUP(_xlpm.Tier, 'Cloud.gov Tiers'!$E$10:$F$28, 2, FALSE))</f>
+        <v>Femto</v>
+      </c>
+      <c r="C5" s="76">
+        <f>VLOOKUP(Table_112[[#This Row],[Tier Name]], 'Cloud.gov Tiers'!A11:B27, 2,FALSE)-Table_112[[#This Row],[Credits]]</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="77">
+        <f>IF(B5="Custom", ROUNDUP(A5/1000,0)*'Cloud.gov Tiers'!$H$28, VLOOKUP(B5, 'Cloud.gov Tiers'!$F$11:$H$27, 3, FALSE))</f>
+        <v>30000</v>
+      </c>
+      <c r="E5" s="77">
+        <f>C15</f>
+        <v>2500</v>
+      </c>
+      <c r="F5" s="84">
+        <f>D5+E5</f>
+        <v>32500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="M8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="85">
+        <v>12</v>
+      </c>
+      <c r="C10" s="12">
+        <f>B10*'Cloud.gov Tiers'!B3</f>
+        <v>36</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="G10" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="40">
+        <v>100</v>
+      </c>
+      <c r="J10" s="85">
+        <v>101</v>
+      </c>
+      <c r="K10" s="42">
+        <f>ROUNDUP(Table_315[[#This Row],[Quantity (GB)]]/Table_315[[#This Row],[GB per credit]],0)</f>
+        <v>2</v>
+      </c>
+      <c r="M10" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="40">
+        <f>'AWS Service Prices'!K5*'AWS Service Prices'!M5</f>
+        <v>400</v>
+      </c>
+      <c r="R10" s="85">
+        <v>401</v>
+      </c>
+      <c r="S10" s="42">
+        <f>ROUNDUP(Table_416[[#This Row],[Quantity (GB)]]/Table_416[[#This Row],[GB per credit]],0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="4"/>
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="E13" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="47" t="str">
+        <f t="array" ref="E14:I43">AWSRdsServicePrices</f>
+        <v>AWS RDS</v>
+      </c>
+      <c r="F14" s="48" t="str">
+        <v>micro-psql</v>
+      </c>
+      <c r="G14" s="48" t="str">
+        <v>db.t3.micro</v>
+      </c>
+      <c r="H14" s="48">
+        <v>1</v>
+      </c>
+      <c r="I14" s="48">
+        <v>1</v>
+      </c>
+      <c r="J14" s="20">
+        <v>2</v>
+      </c>
+      <c r="K14" s="90">
+        <f>I14*J14</f>
+        <v>2</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="22">
+        <v>250</v>
+      </c>
+      <c r="B15" s="86">
+        <v>10</v>
+      </c>
+      <c r="C15" s="23">
+        <f>A15*B15</f>
+        <v>2500</v>
+      </c>
+      <c r="E15" s="24" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F15" s="25" t="str">
+        <v>micro-psql-redundant</v>
+      </c>
+      <c r="G15" s="25" t="str">
+        <v>db.t3.micro</v>
+      </c>
+      <c r="H15" s="25">
+        <v>1</v>
+      </c>
+      <c r="I15" s="25">
+        <v>2</v>
+      </c>
+      <c r="J15" s="35">
+        <v>0</v>
+      </c>
+      <c r="K15" s="90">
+        <f t="shared" ref="K15:K43" si="0">I15*J15</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="N15" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="O15" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="P15" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q15" s="40">
+        <f>'AWS Service Prices'!K4*'AWS Service Prices'!M4</f>
+        <v>100</v>
+      </c>
+      <c r="R15" s="85">
+        <v>0</v>
+      </c>
+      <c r="S15" s="42">
+        <f>ROUNDUP(Table_618[[#This Row],[Quantity (GB)]]/Table_618[[#This Row],[GB per credit]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E16" s="47" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F16" s="48" t="str">
+        <v>small-psql</v>
+      </c>
+      <c r="G16" s="48" t="str">
+        <v>db.t3.small</v>
+      </c>
+      <c r="H16" s="48">
+        <v>1</v>
+      </c>
+      <c r="I16" s="48">
+        <v>2</v>
+      </c>
+      <c r="J16" s="35">
+        <v>0</v>
+      </c>
+      <c r="K16" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="24" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F17" s="25" t="str">
+        <v>small-psql-redundant</v>
+      </c>
+      <c r="G17" s="25" t="str">
+        <v>db.t3.small</v>
+      </c>
+      <c r="H17" s="25">
+        <v>1</v>
+      </c>
+      <c r="I17" s="25">
+        <v>4</v>
+      </c>
+      <c r="J17" s="35">
+        <v>1</v>
+      </c>
+      <c r="K17" s="90">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="47" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F18" s="48" t="str">
+        <v>medium-psql</v>
+      </c>
+      <c r="G18" s="48" t="str">
+        <v>db.t3.medium</v>
+      </c>
+      <c r="H18" s="48">
+        <v>1</v>
+      </c>
+      <c r="I18" s="48">
+        <v>4</v>
+      </c>
+      <c r="J18" s="35">
+        <v>0</v>
+      </c>
+      <c r="K18" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="N18" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="O18" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="P18" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q18" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="R18" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="S18" s="46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="31">
+        <f t="array" ref="B19">'Example worksheet'!$S$10</f>
+        <v>2</v>
+      </c>
+      <c r="E19" s="24" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F19" s="25" t="str">
+        <v>medium-psql-redundant</v>
+      </c>
+      <c r="G19" s="25" t="str">
+        <v>db.t3.medium</v>
+      </c>
+      <c r="H19" s="25">
+        <v>1</v>
+      </c>
+      <c r="I19" s="25">
+        <v>8</v>
+      </c>
+      <c r="J19" s="35">
+        <v>0</v>
+      </c>
+      <c r="K19" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="47" t="str" cm="1">
+        <f t="array" ref="M19:Q29">AwsOpensearchPrices</f>
+        <v>AWS OpenSearch</v>
+      </c>
+      <c r="N19" s="48" t="str">
+        <v>es-dev</v>
+      </c>
+      <c r="O19" s="48" t="str">
+        <v>t3.small.search</v>
+      </c>
+      <c r="P19" s="48">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="48">
+        <v>2</v>
+      </c>
+      <c r="R19" s="32">
+        <v>0</v>
+      </c>
+      <c r="S19" s="21">
+        <f>R19*Q19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="34">
+        <f t="array" ref="B20">SUM(K14:K43) + 'Example worksheet'!$K$10</f>
+        <v>8</v>
+      </c>
+      <c r="E20" s="47" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F20" s="48" t="str">
+        <v>medium-gp-psql</v>
+      </c>
+      <c r="G20" s="48" t="str">
+        <v>db.m5.large</v>
+      </c>
+      <c r="H20" s="48">
+        <v>1</v>
+      </c>
+      <c r="I20" s="48">
+        <v>10</v>
+      </c>
+      <c r="J20" s="35">
+        <v>0</v>
+      </c>
+      <c r="K20" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="24" t="str">
+        <v>AWS OpenSearch</v>
+      </c>
+      <c r="N20" s="25" t="str">
+        <v>es-medium</v>
+      </c>
+      <c r="O20" s="25" t="str">
+        <v>c5.large.search</v>
+      </c>
+      <c r="P20" s="25">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="25">
+        <v>34</v>
+      </c>
+      <c r="R20" s="38">
+        <v>0</v>
+      </c>
+      <c r="S20" s="21">
+        <f t="shared" ref="S20:S29" si="1">R20*Q20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="31">
+        <f>'Example worksheet'!$S$15+SUM(S19:S29)</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="24" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F21" s="25" t="str">
+        <v>medium-gp-psql-redundant</v>
+      </c>
+      <c r="G21" s="25" t="str">
+        <v>db.m5.large</v>
+      </c>
+      <c r="H21" s="25">
+        <v>1</v>
+      </c>
+      <c r="I21" s="25">
+        <v>20</v>
+      </c>
+      <c r="J21" s="35">
+        <v>0</v>
+      </c>
+      <c r="K21" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="47" t="str">
+        <v>AWS OpenSearch</v>
+      </c>
+      <c r="N21" s="48" t="str">
+        <v>es-medium-ha</v>
+      </c>
+      <c r="O21" s="48" t="str">
+        <v>c5.large.search</v>
+      </c>
+      <c r="P21" s="48">
+        <v>7</v>
+      </c>
+      <c r="Q21" s="48">
+        <v>48</v>
+      </c>
+      <c r="R21" s="38">
+        <v>0</v>
+      </c>
+      <c r="S21" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="34">
+        <f>SUM(S33:S37)</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="47" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F22" s="48" t="str">
+        <v>large-gp-psql</v>
+      </c>
+      <c r="G22" s="48" t="str">
+        <v>db.m5.large</v>
+      </c>
+      <c r="H22" s="48">
+        <v>1</v>
+      </c>
+      <c r="I22" s="48">
+        <v>10</v>
+      </c>
+      <c r="J22" s="35">
+        <v>0</v>
+      </c>
+      <c r="K22" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="24" t="str">
+        <v>AWS OpenSearch</v>
+      </c>
+      <c r="N22" s="25" t="str">
+        <v>es-large</v>
+      </c>
+      <c r="O22" s="25" t="str">
+        <v>c5.xlarge.search</v>
+      </c>
+      <c r="P22" s="25">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="25">
+        <v>69</v>
+      </c>
+      <c r="R22" s="38">
+        <v>0</v>
+      </c>
+      <c r="S22" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="37">
+        <f>SUM(Table_820[Credits])</f>
+        <v>2</v>
+      </c>
+      <c r="E23" s="24" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F23" s="25" t="str">
+        <v>large-gp-psql-redundant</v>
+      </c>
+      <c r="G23" s="25" t="str">
+        <v>db.m5.large</v>
+      </c>
+      <c r="H23" s="25">
+        <v>1</v>
+      </c>
+      <c r="I23" s="25">
+        <v>20</v>
+      </c>
+      <c r="J23" s="35">
+        <v>0</v>
+      </c>
+      <c r="K23" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="47" t="str">
+        <v>AWS OpenSearch</v>
+      </c>
+      <c r="N23" s="48" t="str">
+        <v>es-large-ha</v>
+      </c>
+      <c r="O23" s="48" t="str">
+        <v>c5.xlarge.search</v>
+      </c>
+      <c r="P23" s="48">
+        <v>7</v>
+      </c>
+      <c r="Q23" s="48">
+        <v>96</v>
+      </c>
+      <c r="R23" s="38">
+        <v>0</v>
+      </c>
+      <c r="S23" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E24" s="47" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F24" s="48" t="str">
+        <v>xlarge-gp-psql</v>
+      </c>
+      <c r="G24" s="48" t="str">
+        <v>db.m5.xlarge</v>
+      </c>
+      <c r="H24" s="48">
+        <v>1</v>
+      </c>
+      <c r="I24" s="48">
+        <v>20</v>
+      </c>
+      <c r="J24" s="35">
+        <v>0</v>
+      </c>
+      <c r="K24" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="24" t="str">
+        <v>AWS OpenSearch</v>
+      </c>
+      <c r="N24" s="25" t="str">
+        <v>es-xlarge</v>
+      </c>
+      <c r="O24" s="25" t="str">
+        <v>c5.2xlarge.search</v>
+      </c>
+      <c r="P24" s="25">
+        <v>5</v>
+      </c>
+      <c r="Q24" s="25">
+        <v>137</v>
+      </c>
+      <c r="R24" s="38">
+        <v>0</v>
+      </c>
+      <c r="S24" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E25" s="24" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F25" s="25" t="str">
+        <v>xlarge-gp-psql-redundant</v>
+      </c>
+      <c r="G25" s="25" t="str">
+        <v>db.m5.xlarge</v>
+      </c>
+      <c r="H25" s="25">
+        <v>1</v>
+      </c>
+      <c r="I25" s="25">
+        <v>39</v>
+      </c>
+      <c r="J25" s="35">
+        <v>0</v>
+      </c>
+      <c r="K25" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="47" t="str">
+        <v>AWS OpenSearch</v>
+      </c>
+      <c r="N25" s="48" t="str">
+        <v>es-xlarge-ha</v>
+      </c>
+      <c r="O25" s="48" t="str">
+        <v>c5.2xlarge.search</v>
+      </c>
+      <c r="P25" s="48">
+        <v>7</v>
+      </c>
+      <c r="Q25" s="48">
+        <v>192</v>
+      </c>
+      <c r="R25" s="38">
+        <v>0</v>
+      </c>
+      <c r="S25" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="E26" s="47" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F26" s="48" t="str">
+        <v>2xlarge-gp-psql</v>
+      </c>
+      <c r="G26" s="48" t="str">
+        <v>db.m5.2xlarge</v>
+      </c>
+      <c r="H26" s="48">
+        <v>1</v>
+      </c>
+      <c r="I26" s="48">
+        <v>39</v>
+      </c>
+      <c r="J26" s="35">
+        <v>0</v>
+      </c>
+      <c r="K26" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="24" t="str">
+        <v>AWS OpenSearch</v>
+      </c>
+      <c r="N26" s="25" t="str">
+        <v>es-2xlarge-gp</v>
+      </c>
+      <c r="O26" s="25" t="str">
+        <v>m5.2xlarge.search</v>
+      </c>
+      <c r="P26" s="25">
+        <v>5</v>
+      </c>
+      <c r="Q26" s="25">
+        <v>163</v>
+      </c>
+      <c r="R26" s="38">
+        <v>0</v>
+      </c>
+      <c r="S26" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="24" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F27" s="25" t="str">
+        <v>2xlarge-gp-psql-redundant</v>
+      </c>
+      <c r="G27" s="25" t="str">
+        <v>db.m5.2xlarge</v>
+      </c>
+      <c r="H27" s="25">
+        <v>1</v>
+      </c>
+      <c r="I27" s="25">
+        <v>78</v>
+      </c>
+      <c r="J27" s="35">
+        <v>0</v>
+      </c>
+      <c r="K27" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="47" t="str">
+        <v>AWS OpenSearch</v>
+      </c>
+      <c r="N27" s="48" t="str">
+        <v>es-2xlarge-gp-ha</v>
+      </c>
+      <c r="O27" s="48" t="str">
+        <v>m5.2xlarge.search</v>
+      </c>
+      <c r="P27" s="48">
+        <v>7</v>
+      </c>
+      <c r="Q27" s="48">
+        <v>228</v>
+      </c>
+      <c r="R27" s="38">
+        <v>0</v>
+      </c>
+      <c r="S27" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="47" t="str">
+        <f t="array" ref="A28:B35">CloudGovNoCostServices</f>
+        <v>External Domain</v>
+      </c>
+      <c r="B28" s="21" t="str">
+        <v>cdn-route</v>
+      </c>
+      <c r="E28" s="47" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F28" s="48" t="str">
+        <v>xlarge-gp-psql-m6</v>
+      </c>
+      <c r="G28" s="48" t="str">
+        <v>db.m6g.xlarge</v>
+      </c>
+      <c r="H28" s="48">
+        <v>1</v>
+      </c>
+      <c r="I28" s="48">
+        <v>17</v>
+      </c>
+      <c r="J28" s="35">
+        <v>0</v>
+      </c>
+      <c r="K28" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="24" t="str">
+        <v>AWS OpenSearch</v>
+      </c>
+      <c r="N28" s="25" t="str">
+        <v>es-4xlarge-gp</v>
+      </c>
+      <c r="O28" s="25" t="str">
+        <v>m5.4xlarge.search</v>
+      </c>
+      <c r="P28" s="25">
+        <v>5</v>
+      </c>
+      <c r="Q28" s="25">
+        <v>326</v>
+      </c>
+      <c r="R28" s="38">
+        <v>0</v>
+      </c>
+      <c r="S28" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="24" t="str">
+        <v>External Domain</v>
+      </c>
+      <c r="B29" s="27" t="str">
+        <v>custom-domain</v>
+      </c>
+      <c r="E29" s="24" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F29" s="25" t="str">
+        <v>xlarge-gp-psql-m6-redundant</v>
+      </c>
+      <c r="G29" s="25" t="str">
+        <v>db.m6g.xlarge</v>
+      </c>
+      <c r="H29" s="25">
+        <v>1</v>
+      </c>
+      <c r="I29" s="25">
+        <v>34</v>
+      </c>
+      <c r="J29" s="35">
+        <v>0</v>
+      </c>
+      <c r="K29" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="39" t="str">
+        <v>AWS OpenSearch</v>
+      </c>
+      <c r="N29" s="40" t="str">
+        <v>es-4xlarge-gp-ha</v>
+      </c>
+      <c r="O29" s="40" t="str">
+        <v>m5.4xlarge.search</v>
+      </c>
+      <c r="P29" s="40">
+        <v>7</v>
+      </c>
+      <c r="Q29" s="40">
+        <v>456</v>
+      </c>
+      <c r="R29" s="41">
+        <v>0</v>
+      </c>
+      <c r="S29" s="91">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T29" s="92"/>
+    </row>
+    <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="47" t="str">
+        <v>External Domain</v>
+      </c>
+      <c r="B30" s="21" t="str">
+        <v>domain</v>
+      </c>
+      <c r="E30" s="47" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F30" s="48" t="str">
+        <v>micro-mysql</v>
+      </c>
+      <c r="G30" s="48" t="str">
+        <v>db.t3.micro</v>
+      </c>
+      <c r="H30" s="48">
+        <v>1</v>
+      </c>
+      <c r="I30" s="48">
+        <v>1</v>
+      </c>
+      <c r="J30" s="43">
+        <v>0</v>
+      </c>
+      <c r="K30" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y30" s="29"/>
+    </row>
+    <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="24" t="str">
+        <v>External Domain</v>
+      </c>
+      <c r="B31" s="27" t="str">
+        <v>domain-with-cdn</v>
+      </c>
+      <c r="E31" s="24" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F31" s="25" t="str">
+        <v>micro-mysql-redundant</v>
+      </c>
+      <c r="G31" s="25" t="str">
+        <v>db.t3.micro</v>
+      </c>
+      <c r="H31" s="25">
+        <v>1</v>
+      </c>
+      <c r="I31" s="25">
+        <v>2</v>
+      </c>
+      <c r="J31" s="35">
+        <v>0</v>
+      </c>
+      <c r="K31" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="47" t="str">
+        <v>UAA Service Account</v>
+      </c>
+      <c r="B32" s="21" t="str">
+        <v>oauth-client</v>
+      </c>
+      <c r="E32" s="47" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F32" s="48" t="str">
+        <v>small-mysql</v>
+      </c>
+      <c r="G32" s="48" t="str">
+        <v>db.t3.small</v>
+      </c>
+      <c r="H32" s="48">
+        <v>1</v>
+      </c>
+      <c r="I32" s="48">
+        <v>2</v>
+      </c>
+      <c r="J32" s="35">
+        <v>0</v>
+      </c>
+      <c r="K32" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="N32" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="O32" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="P32" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q32" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="R32" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="S32" s="46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="24" t="str">
+        <v>UAA Service Account</v>
+      </c>
+      <c r="B33" s="27" t="str">
+        <v>space-auditor</v>
+      </c>
+      <c r="E33" s="24" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F33" s="25" t="str">
+        <v>small-mysql-redundant</v>
+      </c>
+      <c r="G33" s="25" t="str">
+        <v>db.t3.small</v>
+      </c>
+      <c r="H33" s="25">
+        <v>1</v>
+      </c>
+      <c r="I33" s="25">
+        <v>4</v>
+      </c>
+      <c r="J33" s="35">
+        <v>0</v>
+      </c>
+      <c r="K33" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="47" t="str" cm="1">
+        <f t="array" ref="M33:Q37">AwsElasticCachePrices</f>
+        <v>AWS ElastiCache</v>
+      </c>
+      <c r="N33" s="48" t="str">
+        <v>redis-dev</v>
+      </c>
+      <c r="O33" s="48" t="str">
+        <v>cache.t3.micro</v>
+      </c>
+      <c r="P33" s="48">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="88">
+        <v>1</v>
+      </c>
+      <c r="R33" s="50">
+        <v>0</v>
+      </c>
+      <c r="S33" s="21">
+        <f>R33*Q33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="47" t="str">
+        <v>UAA Service Account</v>
+      </c>
+      <c r="B34" s="21" t="str">
+        <v>space-deployer</v>
+      </c>
+      <c r="E34" s="47" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F34" s="48" t="str">
+        <v>medium-mysql</v>
+      </c>
+      <c r="G34" s="48" t="str">
+        <v>db.t3.medium</v>
+      </c>
+      <c r="H34" s="48">
+        <v>1</v>
+      </c>
+      <c r="I34" s="48">
+        <v>4</v>
+      </c>
+      <c r="J34" s="35">
+        <v>0</v>
+      </c>
+      <c r="K34" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M34" s="24" t="str">
+        <v>AWS ElastiCache</v>
+      </c>
+      <c r="N34" s="25" t="str">
+        <v>redis-3node</v>
+      </c>
+      <c r="O34" s="25" t="str">
+        <v>cache.t3.micro</v>
+      </c>
+      <c r="P34" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q34" s="88">
+        <v>2</v>
+      </c>
+      <c r="R34" s="38">
+        <v>0</v>
+      </c>
+      <c r="S34" s="21">
+        <f t="shared" ref="S34:S37" si="2">R34*Q34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="24" t="str">
+        <v>Autoscaler</v>
+      </c>
+      <c r="B35" s="27" t="str">
+        <v>autoscaler-free-plan</v>
+      </c>
+      <c r="E35" s="24" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F35" s="25" t="str">
+        <v>medium-mysql-redundant</v>
+      </c>
+      <c r="G35" s="25" t="str">
+        <v>db.t3.medium</v>
+      </c>
+      <c r="H35" s="25">
+        <v>1</v>
+      </c>
+      <c r="I35" s="25">
+        <v>7</v>
+      </c>
+      <c r="J35" s="35">
+        <v>0</v>
+      </c>
+      <c r="K35" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M35" s="47" t="str">
+        <v>AWS ElastiCache</v>
+      </c>
+      <c r="N35" s="48" t="str">
+        <v>redis-5node</v>
+      </c>
+      <c r="O35" s="48" t="str">
+        <v>cache.t3.micro</v>
+      </c>
+      <c r="P35" s="48">
+        <v>5</v>
+      </c>
+      <c r="Q35" s="88">
+        <v>4</v>
+      </c>
+      <c r="R35" s="38">
+        <v>0</v>
+      </c>
+      <c r="S35" s="21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" s="44"/>
+      <c r="E36" s="47" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F36" s="48" t="str">
+        <v>medium-gp-mysql</v>
+      </c>
+      <c r="G36" s="48" t="str">
+        <v>db.m5.large</v>
+      </c>
+      <c r="H36" s="48">
+        <v>1</v>
+      </c>
+      <c r="I36" s="48">
+        <v>9</v>
+      </c>
+      <c r="J36" s="35">
+        <v>0</v>
+      </c>
+      <c r="K36" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="24" t="str">
+        <v>AWS ElastiCache</v>
+      </c>
+      <c r="N36" s="25" t="str">
+        <v>redis-3node-large</v>
+      </c>
+      <c r="O36" s="25" t="str">
+        <v>cache.t3.small</v>
+      </c>
+      <c r="P36" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q36" s="88">
+        <v>5</v>
+      </c>
+      <c r="R36" s="38">
+        <v>0</v>
+      </c>
+      <c r="S36" s="21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E37" s="24" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F37" s="25" t="str">
+        <v>medium-gp-mysql-redundant</v>
+      </c>
+      <c r="G37" s="25" t="str">
+        <v>db.m5.large</v>
+      </c>
+      <c r="H37" s="25">
+        <v>1</v>
+      </c>
+      <c r="I37" s="25">
+        <v>19</v>
+      </c>
+      <c r="J37" s="35">
+        <v>0</v>
+      </c>
+      <c r="K37" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M37" s="39" t="str">
+        <v>AWS ElastiCache</v>
+      </c>
+      <c r="N37" s="40" t="str">
+        <v>redis-5node-large</v>
+      </c>
+      <c r="O37" s="40" t="str">
+        <v>cache.t3.small</v>
+      </c>
+      <c r="P37" s="40">
+        <v>5</v>
+      </c>
+      <c r="Q37" s="89">
+        <v>8</v>
+      </c>
+      <c r="R37" s="45">
+        <v>0</v>
+      </c>
+      <c r="S37" s="91">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E38" s="47" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F38" s="48" t="str">
+        <v>large-gp-mysql</v>
+      </c>
+      <c r="G38" s="48" t="str">
+        <v>db.m5.large</v>
+      </c>
+      <c r="H38" s="48">
+        <v>1</v>
+      </c>
+      <c r="I38" s="48">
+        <v>9</v>
+      </c>
+      <c r="J38" s="35">
+        <v>0</v>
+      </c>
+      <c r="K38" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="102" t="s">
+        <v>183</v>
+      </c>
+      <c r="B39" s="103" t="s">
+        <v>184</v>
+      </c>
+      <c r="C39" s="104" t="s">
+        <v>185</v>
+      </c>
+      <c r="E39" s="24" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F39" s="25" t="str">
+        <v>large-gp-mysql-redundant</v>
+      </c>
+      <c r="G39" s="25" t="str">
+        <v>db.m5.large</v>
+      </c>
+      <c r="H39" s="25">
+        <v>1</v>
+      </c>
+      <c r="I39" s="25">
+        <v>19</v>
+      </c>
+      <c r="J39" s="35">
+        <v>0</v>
+      </c>
+      <c r="K39" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="105">
+        <v>1</v>
+      </c>
+      <c r="B40" s="101">
+        <v>45748</v>
+      </c>
+      <c r="C40" s="100" t="s">
+        <v>189</v>
+      </c>
+      <c r="E40" s="47" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F40" s="48" t="str">
+        <v>xlarge-gp-mysql</v>
+      </c>
+      <c r="G40" s="48" t="str">
+        <v>db.m5.xlarge</v>
+      </c>
+      <c r="H40" s="48">
+        <v>1</v>
+      </c>
+      <c r="I40" s="48">
+        <v>19</v>
+      </c>
+      <c r="J40" s="35">
+        <v>0</v>
+      </c>
+      <c r="K40" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M40" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="N40" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="O40" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="P40" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q40" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="R40" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="S40" s="95" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="105">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B41" s="101">
+        <v>45749</v>
+      </c>
+      <c r="C41" s="100" t="s">
+        <v>186</v>
+      </c>
+      <c r="E41" s="24" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F41" s="25" t="str">
+        <v>xlarge-gp-mysql-redundant</v>
+      </c>
+      <c r="G41" s="25" t="str">
+        <v>db.m5.xlarge</v>
+      </c>
+      <c r="H41" s="25">
+        <v>1</v>
+      </c>
+      <c r="I41" s="25">
+        <v>37</v>
+      </c>
+      <c r="J41" s="35">
+        <v>0</v>
+      </c>
+      <c r="K41" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M41" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="N41" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="O41" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="P41" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q41" s="88">
+        <f>'AWS Service Prices'!K6*'AWS Service Prices'!M6</f>
+        <v>150000</v>
+      </c>
+      <c r="R41" s="93">
+        <v>1000</v>
+      </c>
+      <c r="S41" s="97">
+        <f>ROUNDUP(Table_820[[#This Row],[Quantity]]/Table_820[[#This Row],[Units/Credit]],0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="105"/>
+      <c r="C42" s="100" t="s">
+        <v>187</v>
+      </c>
+      <c r="E42" s="47" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F42" s="48" t="str">
+        <v>medium-oracle-se2</v>
+      </c>
+      <c r="G42" s="48" t="str">
+        <v>db.t3.medium</v>
+      </c>
+      <c r="H42" s="48">
+        <v>1</v>
+      </c>
+      <c r="I42" s="48">
+        <v>7</v>
+      </c>
+      <c r="J42" s="35">
+        <v>0</v>
+      </c>
+      <c r="K42" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M42" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="N42" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="O42" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="P42" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q42" s="88">
+        <f>'AWS Service Prices'!K7*'AWS Service Prices'!M7</f>
+        <v>120</v>
+      </c>
+      <c r="R42" s="94">
+        <v>2</v>
+      </c>
+      <c r="S42" s="96">
+        <f>ROUNDUP(Table_820[[#This Row],[Quantity]]/Table_820[[#This Row],[Units/Credit]],0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="105"/>
+      <c r="C43" s="100" t="s">
+        <v>188</v>
+      </c>
+      <c r="E43" s="54" t="str">
+        <v>AWS RDS</v>
+      </c>
+      <c r="F43" s="55" t="str">
+        <v>large-gp-sqlserver-se</v>
+      </c>
+      <c r="G43" s="55" t="str">
+        <v>db.m5.large</v>
+      </c>
+      <c r="H43" s="55">
+        <v>1</v>
+      </c>
+      <c r="I43" s="55">
+        <v>46</v>
+      </c>
+      <c r="J43" s="56">
+        <v>0</v>
+      </c>
+      <c r="K43" s="99">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q43" s="98"/>
+    </row>
+    <row r="44" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="105">
+        <v>1.2</v>
+      </c>
+      <c r="B44" s="101">
+        <v>45756</v>
+      </c>
+      <c r="C44" s="106" t="s">
+        <v>190</v>
+      </c>
+      <c r="J44" s="4"/>
+    </row>
+    <row r="45" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="105">
+        <v>1.3</v>
+      </c>
+      <c r="B45" s="101">
+        <v>45757</v>
+      </c>
+      <c r="C45" s="106" t="s">
+        <v>191</v>
+      </c>
+      <c r="J45" s="4"/>
+    </row>
+    <row r="46" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="105"/>
+      <c r="J46" s="4"/>
+    </row>
+    <row r="47" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="105"/>
+      <c r="J47" s="4"/>
+    </row>
+    <row r="48" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="105"/>
+      <c r="J48" s="4"/>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="105"/>
+      <c r="J49" s="4"/>
+    </row>
+    <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="105"/>
+      <c r="J50" s="4"/>
+    </row>
+    <row r="51" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J51" s="4"/>
+    </row>
+    <row r="52" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J52" s="4"/>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J53" s="4"/>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J54" s="4"/>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J55" s="4"/>
+    </row>
+    <row r="56" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J56" s="4"/>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J57" s="4"/>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J58" s="4"/>
+    </row>
+    <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J59" s="4"/>
+    </row>
+    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J60" s="4"/>
+    </row>
+    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J61" s="4"/>
+    </row>
+    <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J62" s="4"/>
+    </row>
+    <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J63" s="4"/>
+    </row>
+    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J64" s="4"/>
+    </row>
+    <row r="65" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J65" s="4"/>
+    </row>
+    <row r="66" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J66" s="4"/>
+    </row>
+    <row r="67" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J67" s="4"/>
+    </row>
+    <row r="68" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J68" s="4"/>
+    </row>
+    <row r="69" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J69" s="4"/>
+    </row>
+    <row r="70" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J70" s="4"/>
+    </row>
+    <row r="71" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J71" s="4"/>
+    </row>
+    <row r="72" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J72" s="4"/>
+    </row>
+    <row r="73" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J73" s="4"/>
+    </row>
+    <row r="74" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J74" s="4"/>
+    </row>
+    <row r="75" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J75" s="4"/>
+    </row>
+    <row r="76" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J76" s="4"/>
+    </row>
+    <row r="77" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J77" s="4"/>
+    </row>
+    <row r="78" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J78" s="4"/>
+    </row>
+    <row r="79" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="80" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B10 J14:J43 B15">
+    <cfRule type="cellIs" dxfId="45" priority="14" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="expression" dxfId="44" priority="6">
+      <formula>$J$10&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14:F43">
+    <cfRule type="expression" dxfId="43" priority="7">
+      <formula>$J14&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10">
+    <cfRule type="cellIs" dxfId="42" priority="8" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N10">
+    <cfRule type="expression" dxfId="41" priority="4">
+      <formula>$R10&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N15">
+    <cfRule type="expression" dxfId="40" priority="5">
+      <formula>$R15&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N19:N29">
+    <cfRule type="expression" dxfId="39" priority="3">
+      <formula>$R19&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N33:N37">
+    <cfRule type="expression" dxfId="38" priority="2">
+      <formula>$R33&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N41:N42">
+    <cfRule type="expression" dxfId="37" priority="1">
+      <formula>$R41&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R10">
+    <cfRule type="cellIs" dxfId="36" priority="10" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R15">
+    <cfRule type="cellIs" dxfId="35" priority="9" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R19:R29">
+    <cfRule type="cellIs" dxfId="34" priority="12" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R33:R37">
+    <cfRule type="cellIs" dxfId="33" priority="11" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R41:R42">
+    <cfRule type="cellIs" dxfId="32" priority="13" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape"/>
+  <tableParts count="9">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update cost estimator spreadsheet
</commit_message>
<xml_diff>
--- a/_assets/documents/cloud-gov-cost-estimator.xlsx
+++ b/_assets/documents/cloud-gov-cost-estimator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markdboyd/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683BB082-E3A7-DA41-81A3-C727EAF70EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6BFDD4-0CDB-4742-8222-F68AE10270B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5583,8 +5583,8 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J29" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P46" sqref="P46"/>
+    <sheetView tabSelected="1" topLeftCell="F19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7327,7 +7327,7 @@
         <v>0</v>
       </c>
       <c r="Q46" s="119">
-        <f>$O$46*$P$46</f>
+        <f>O46*P46</f>
         <v>0</v>
       </c>
       <c r="R46" s="112"/>

</xml_diff>

<commit_message>
update page and spreadsheet to note correct date of last version update for pricing spreadsheet
</commit_message>
<xml_diff>
--- a/_assets/documents/cloud-gov-cost-estimator.xlsx
+++ b/_assets/documents/cloud-gov-cost-estimator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markdboyd/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6BFDD4-0CDB-4742-8222-F68AE10270B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C5E9B5-D04A-0047-B569-6F61061D3C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1834,10 +1834,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1884,12 +1880,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="194">
+  <dxfs count="125">
     <dxf>
       <font>
         <b/>
@@ -2048,13 +2048,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <u/>
@@ -2118,657 +2111,6 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5002,54 +4344,54 @@
   </dxfs>
   <tableStyles count="10">
     <tableStyle name="Worksheet-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="193"/>
-      <tableStyleElement type="firstRowStripe" dxfId="192"/>
-      <tableStyleElement type="secondRowStripe" dxfId="191"/>
+      <tableStyleElement type="headerRow" dxfId="124"/>
+      <tableStyleElement type="firstRowStripe" dxfId="123"/>
+      <tableStyleElement type="secondRowStripe" dxfId="122"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="190"/>
-      <tableStyleElement type="firstRowStripe" dxfId="189"/>
-      <tableStyleElement type="secondRowStripe" dxfId="188"/>
+      <tableStyleElement type="headerRow" dxfId="121"/>
+      <tableStyleElement type="firstRowStripe" dxfId="120"/>
+      <tableStyleElement type="secondRowStripe" dxfId="119"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="headerRow" dxfId="187"/>
-      <tableStyleElement type="firstRowStripe" dxfId="186"/>
-      <tableStyleElement type="secondRowStripe" dxfId="185"/>
+      <tableStyleElement type="headerRow" dxfId="118"/>
+      <tableStyleElement type="firstRowStripe" dxfId="117"/>
+      <tableStyleElement type="secondRowStripe" dxfId="116"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 4" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
-      <tableStyleElement type="headerRow" dxfId="184"/>
-      <tableStyleElement type="firstRowStripe" dxfId="183"/>
-      <tableStyleElement type="secondRowStripe" dxfId="182"/>
+      <tableStyleElement type="headerRow" dxfId="115"/>
+      <tableStyleElement type="firstRowStripe" dxfId="114"/>
+      <tableStyleElement type="secondRowStripe" dxfId="113"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 5" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
-      <tableStyleElement type="headerRow" dxfId="181"/>
-      <tableStyleElement type="firstRowStripe" dxfId="180"/>
-      <tableStyleElement type="secondRowStripe" dxfId="179"/>
+      <tableStyleElement type="headerRow" dxfId="112"/>
+      <tableStyleElement type="firstRowStripe" dxfId="111"/>
+      <tableStyleElement type="secondRowStripe" dxfId="110"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 6" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
-      <tableStyleElement type="headerRow" dxfId="178"/>
-      <tableStyleElement type="firstRowStripe" dxfId="177"/>
-      <tableStyleElement type="secondRowStripe" dxfId="176"/>
+      <tableStyleElement type="headerRow" dxfId="109"/>
+      <tableStyleElement type="firstRowStripe" dxfId="108"/>
+      <tableStyleElement type="secondRowStripe" dxfId="107"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 7" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF06000000}">
-      <tableStyleElement type="headerRow" dxfId="175"/>
-      <tableStyleElement type="firstRowStripe" dxfId="174"/>
-      <tableStyleElement type="secondRowStripe" dxfId="173"/>
+      <tableStyleElement type="headerRow" dxfId="106"/>
+      <tableStyleElement type="firstRowStripe" dxfId="105"/>
+      <tableStyleElement type="secondRowStripe" dxfId="104"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 8" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF07000000}">
-      <tableStyleElement type="headerRow" dxfId="172"/>
-      <tableStyleElement type="firstRowStripe" dxfId="171"/>
-      <tableStyleElement type="secondRowStripe" dxfId="170"/>
+      <tableStyleElement type="headerRow" dxfId="103"/>
+      <tableStyleElement type="firstRowStripe" dxfId="102"/>
+      <tableStyleElement type="secondRowStripe" dxfId="101"/>
     </tableStyle>
     <tableStyle name="Cloud.gov Tiers-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF08000000}">
-      <tableStyleElement type="headerRow" dxfId="169"/>
-      <tableStyleElement type="firstRowStripe" dxfId="168"/>
-      <tableStyleElement type="secondRowStripe" dxfId="167"/>
+      <tableStyleElement type="headerRow" dxfId="100"/>
+      <tableStyleElement type="firstRowStripe" dxfId="99"/>
+      <tableStyleElement type="secondRowStripe" dxfId="98"/>
     </tableStyle>
     <tableStyle name="Cloud.gov Tiers-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF09000000}">
-      <tableStyleElement type="headerRow" dxfId="166"/>
-      <tableStyleElement type="firstRowStripe" dxfId="165"/>
-      <tableStyleElement type="secondRowStripe" dxfId="164"/>
+      <tableStyleElement type="headerRow" dxfId="97"/>
+      <tableStyleElement type="firstRowStripe" dxfId="96"/>
+      <tableStyleElement type="secondRowStripe" dxfId="95"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -5066,20 +4408,20 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A4:F5">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Credits" dataDxfId="163"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tier Name" dataDxfId="162">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Credits" dataDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tier Name" dataDxfId="93">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.Tier, VLOOKUP(MIN(IF('Cloud.gov Tiers'!$B$11:$B$28&gt;=A5, 'Cloud.gov Tiers'!$B$11:$B$28)), 'Cloud.gov Tiers'!$B$11:$E$28, 4, FALSE), VLOOKUP(_xlpm.Tier, 'Cloud.gov Tiers'!$E$10:$F$28, 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Credits Remaining_x000a_in Tier" dataDxfId="161">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Credits Remaining_x000a_in Tier" dataDxfId="92">
       <calculatedColumnFormula>VLOOKUP(Table_1[[#This Row],[Tier Name]], 'Cloud.gov Tiers'!A11:B27, 2,FALSE)-Table_1[[#This Row],[Credits]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Yearly_x000a_Platform Total" dataDxfId="160">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Yearly_x000a_Platform Total" dataDxfId="91">
       <calculatedColumnFormula>IF(B5="Custom", ROUNDUP(A5/1000,0)*'Cloud.gov Tiers'!$H$28, VLOOKUP(B5, 'Cloud.gov Tiers'!$F$11:$H$27, 3, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Support Total" dataDxfId="159">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Support Total" dataDxfId="90">
       <calculatedColumnFormula>C15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name=" YearlyTotal Cost" dataDxfId="158">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name=" YearlyTotal Cost" dataDxfId="89">
       <calculatedColumnFormula>D5+E5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5116,22 +4458,22 @@
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{4C37D040-F691-2C49-BE22-816489BFD4D2}" name="Table_112" displayName="Table_112" ref="A4:F5">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{657244D4-FE4C-D44C-B48B-43E7FA139C6B}" name="Credits" dataDxfId="131">
+    <tableColumn id="1" xr3:uid="{657244D4-FE4C-D44C-B48B-43E7FA139C6B}" name="Credits" dataDxfId="62">
       <calculatedColumnFormula>C10+SUM(B19:B23)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B168D809-F848-8A4F-B241-57C6EF027C29}" name="Tier Name" dataDxfId="130">
+    <tableColumn id="2" xr3:uid="{B168D809-F848-8A4F-B241-57C6EF027C29}" name="Tier Name" dataDxfId="61">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.Tier, VLOOKUP(MIN(IF('Cloud.gov Tiers'!$B$11:$B$28&gt;=A5, 'Cloud.gov Tiers'!$B$11:$B$28)), 'Cloud.gov Tiers'!$B$11:$E$28, 4, FALSE), VLOOKUP(_xlpm.Tier, 'Cloud.gov Tiers'!$E$10:$F$28, 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{172BAC85-F7D2-7D4C-9C26-72C7C85DB56F}" name="Credits Remaining_x000a_in Tier" dataDxfId="129">
+    <tableColumn id="3" xr3:uid="{172BAC85-F7D2-7D4C-9C26-72C7C85DB56F}" name="Credits Remaining_x000a_in Tier" dataDxfId="60">
       <calculatedColumnFormula>VLOOKUP(Table_112[[#This Row],[Tier Name]], 'Cloud.gov Tiers'!A11:B27, 2,FALSE)-Table_112[[#This Row],[Credits]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{19498A2C-21A7-B740-9DD5-D095ED0DD812}" name="Yearly_x000a_Platform Total" dataDxfId="128">
+    <tableColumn id="4" xr3:uid="{19498A2C-21A7-B740-9DD5-D095ED0DD812}" name="Yearly_x000a_Platform Total" dataDxfId="59">
       <calculatedColumnFormula>IF(B5="Custom", ROUNDUP(A5/1000,0)*'Cloud.gov Tiers'!$H$28, VLOOKUP(B5, 'Cloud.gov Tiers'!$F$11:$H$27, 3, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{A475BA76-45A9-EF46-8FAE-2B381389CF6E}" name="Support Total" dataDxfId="127">
+    <tableColumn id="5" xr3:uid="{A475BA76-45A9-EF46-8FAE-2B381389CF6E}" name="Support Total" dataDxfId="58">
       <calculatedColumnFormula>C15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{CFD58EB9-7FC4-3640-859D-34D006952E97}" name=" YearlyTotal Cost" dataDxfId="126">
+    <tableColumn id="6" xr3:uid="{CFD58EB9-7FC4-3640-859D-34D006952E97}" name=" YearlyTotal Cost" dataDxfId="57">
       <calculatedColumnFormula>D5+E5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5143,7 +4485,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{432B26DD-C481-9945-89E7-FEF42FEDB769}" name="Table_214" displayName="Table_214" ref="A9:C10">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8D2D857E-9AA6-5D4F-A4AF-373B7168526E}" name="Resource"/>
-    <tableColumn id="2" xr3:uid="{4FAE5D4B-8591-7D41-A69E-501EE57C6C41}" name="Quantity" dataDxfId="125"/>
+    <tableColumn id="2" xr3:uid="{4FAE5D4B-8591-7D41-A69E-501EE57C6C41}" name="Quantity" dataDxfId="56"/>
     <tableColumn id="3" xr3:uid="{FD66B2C4-D49F-1C43-9A30-DE1F21B9FD5B}" name="Credits">
       <calculatedColumnFormula>B10*'Cloud.gov Tiers'!B3</calculatedColumnFormula>
     </tableColumn>
@@ -5155,13 +4497,13 @@
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{3AE58A18-ABB7-FC4E-9D28-06F1CAA78773}" name="Table_315" displayName="Table_315" ref="E9:K10">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8901DDBE-58BA-8F4F-9D7C-2A2800A70157}" name="Offering" dataDxfId="124"/>
-    <tableColumn id="2" xr3:uid="{3C07AF3B-6C04-4348-A1E4-AEF634AB5F2C}" name="Description" dataDxfId="123"/>
-    <tableColumn id="3" xr3:uid="{50B2B6E3-7A84-CC41-A61F-9E7C70E4AC01}" name="Units" dataDxfId="122"/>
-    <tableColumn id="4" xr3:uid="{99748816-FA07-B948-9F02-BAFA13C63BF0}" name="Dimension" dataDxfId="121"/>
-    <tableColumn id="5" xr3:uid="{B4686AED-FFA8-0F4F-8CF1-A28CBB869F59}" name="GB per credit" dataDxfId="120"/>
-    <tableColumn id="6" xr3:uid="{C47C64B0-2C30-0043-A34C-7F0E810B25DC}" name="Quantity (GB)" dataDxfId="119"/>
-    <tableColumn id="7" xr3:uid="{D0A5DC61-9EB0-294B-94B0-91D19A5D6E7E}" name="Credits" dataDxfId="118">
+    <tableColumn id="1" xr3:uid="{8901DDBE-58BA-8F4F-9D7C-2A2800A70157}" name="Offering" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{3C07AF3B-6C04-4348-A1E4-AEF634AB5F2C}" name="Description" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{50B2B6E3-7A84-CC41-A61F-9E7C70E4AC01}" name="Units" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{99748816-FA07-B948-9F02-BAFA13C63BF0}" name="Dimension" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{B4686AED-FFA8-0F4F-8CF1-A28CBB869F59}" name="GB per credit" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{C47C64B0-2C30-0043-A34C-7F0E810B25DC}" name="Quantity (GB)" dataDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{D0A5DC61-9EB0-294B-94B0-91D19A5D6E7E}" name="Credits" dataDxfId="49">
       <calculatedColumnFormula>ROUNDUP(Table_315[[#This Row],[Quantity (GB)]]/Table_315[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5175,12 +4517,12 @@
     <tableColumn id="1" xr3:uid="{CC812881-5649-1A4C-8C45-49D7808E0D1A}" name="Offering"/>
     <tableColumn id="2" xr3:uid="{46204D59-C3E2-174B-9C58-1DB2BB6988C8}" name="Description"/>
     <tableColumn id="4" xr3:uid="{C3D129A0-D876-D446-9BED-4CE757DA989E}" name="Units"/>
-    <tableColumn id="5" xr3:uid="{8159B7E1-3CBB-384F-9C82-294839F55CB1}" name="Dimension" dataDxfId="117"/>
-    <tableColumn id="3" xr3:uid="{6374D1D7-2C6C-674A-9B2C-B5EA274BAEAC}" name="GB per credit" dataDxfId="116">
+    <tableColumn id="5" xr3:uid="{8159B7E1-3CBB-384F-9C82-294839F55CB1}" name="Dimension" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{6374D1D7-2C6C-674A-9B2C-B5EA274BAEAC}" name="GB per credit" dataDxfId="47">
       <calculatedColumnFormula>'AWS Service Prices'!K5*'AWS Service Prices'!M5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{84537EB8-58A4-A645-9A18-A322EFB5D6C3}" name="Quantity (GB)" dataDxfId="115"/>
-    <tableColumn id="7" xr3:uid="{06CE2B03-0479-2148-9683-4F1675E4317C}" name="Credits" dataDxfId="114">
+    <tableColumn id="6" xr3:uid="{84537EB8-58A4-A645-9A18-A322EFB5D6C3}" name="Quantity (GB)" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{06CE2B03-0479-2148-9683-4F1675E4317C}" name="Credits" dataDxfId="45">
       <calculatedColumnFormula>ROUNDUP(Table_416[[#This Row],[Quantity (GB)]]/Table_416[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5192,7 +4534,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{DD38669A-9AE2-BA49-AF4A-F9D5CEFDB233}" name="Table_517" displayName="Table_517" ref="A14:C15">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E0798FE9-1580-1B43-B088-25897B8976F6}" name="Rate/Hour"/>
-    <tableColumn id="2" xr3:uid="{4F69F05E-31AF-C644-B087-9847D08BB3A0}" name="Hours" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{4F69F05E-31AF-C644-B087-9847D08BB3A0}" name="Hours" dataDxfId="44"/>
     <tableColumn id="3" xr3:uid="{35F99F2C-96B5-1244-8BF2-D8FA71D1A5B2}" name="Total">
       <calculatedColumnFormula>A15*B15</calculatedColumnFormula>
     </tableColumn>
@@ -5202,17 +4544,17 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{53A578BF-BA5A-7843-972B-EBD4EA7AD1DD}" name="Table_618" displayName="Table_618" ref="M14:S15" dataDxfId="112">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{53A578BF-BA5A-7843-972B-EBD4EA7AD1DD}" name="Table_618" displayName="Table_618" ref="M14:S15" dataDxfId="43">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3024083C-5ED0-8D4D-8D1A-D4BD5916AE47}" name="Offering" dataDxfId="111"/>
-    <tableColumn id="2" xr3:uid="{3D92B04D-745E-2A49-991D-C00C27907719}" name="Description" dataDxfId="110"/>
-    <tableColumn id="4" xr3:uid="{50C39022-EBD5-9B42-84DD-C507ED702117}" name="Units" dataDxfId="109"/>
-    <tableColumn id="5" xr3:uid="{9759566D-ABA1-0943-92F2-2B5501002EE3}" name="Dimension" dataDxfId="108"/>
-    <tableColumn id="3" xr3:uid="{4A17BDB6-3CD8-BF43-B5F9-82D2A2C35A0C}" name="GB per credit" dataDxfId="107">
+    <tableColumn id="1" xr3:uid="{3024083C-5ED0-8D4D-8D1A-D4BD5916AE47}" name="Offering" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{3D92B04D-745E-2A49-991D-C00C27907719}" name="Description" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{50C39022-EBD5-9B42-84DD-C507ED702117}" name="Units" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{9759566D-ABA1-0943-92F2-2B5501002EE3}" name="Dimension" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{4A17BDB6-3CD8-BF43-B5F9-82D2A2C35A0C}" name="GB per credit" dataDxfId="38">
       <calculatedColumnFormula>'AWS Service Prices'!K4*'AWS Service Prices'!M4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{056FCEF1-5646-814F-8034-1E8AC53C910D}" name="Quantity (GB)" dataDxfId="106"/>
-    <tableColumn id="7" xr3:uid="{DAEA814F-05EA-764E-8533-FE0EF6F3B132}" name="Credits" dataDxfId="105">
+    <tableColumn id="6" xr3:uid="{056FCEF1-5646-814F-8034-1E8AC53C910D}" name="Quantity (GB)" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{DAEA814F-05EA-764E-8533-FE0EF6F3B132}" name="Credits" dataDxfId="36">
       <calculatedColumnFormula>ROUNDUP(Table_618[[#This Row],[Quantity (GB)]]/Table_618[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5237,11 +4579,11 @@
     <tableColumn id="2" xr3:uid="{B074D0B3-B914-AB4F-8066-81B90B3261D8}" name="Description"/>
     <tableColumn id="4" xr3:uid="{202C8C30-FD4E-6D40-9EBF-642B8C7AE181}" name="Units"/>
     <tableColumn id="5" xr3:uid="{CA6A3A17-2747-AF44-8119-FC05700B8D5C}" name="Dimension"/>
-    <tableColumn id="3" xr3:uid="{C6C6ED4B-9612-3F48-9D18-472E70646A28}" name="Units/Credit" dataDxfId="104">
+    <tableColumn id="3" xr3:uid="{C6C6ED4B-9612-3F48-9D18-472E70646A28}" name="Units/Credit" dataDxfId="35">
       <calculatedColumnFormula>'AWS Service Prices'!K6*'AWS Service Prices'!M6</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{76CCCB3A-2B18-4C42-9DB6-C570AFD6FB75}" name="Quantity"/>
-    <tableColumn id="7" xr3:uid="{A024F374-2C63-444D-95DA-745B84ABCFE7}" name="Credits" dataDxfId="103">
+    <tableColumn id="7" xr3:uid="{A024F374-2C63-444D-95DA-745B84ABCFE7}" name="Credits" dataDxfId="34">
       <calculatedColumnFormula>ROUNDUP(Table_820[[#This Row],[Quantity]]/Table_820[[#This Row],[Units/Credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5253,7 +4595,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A9:C10">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Resource"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Quantity" dataDxfId="157"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Quantity" dataDxfId="88"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Credits"/>
   </tableColumns>
   <tableStyleInfo name="Worksheet-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
@@ -5261,10 +4603,10 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{333F2C22-64BE-8A4A-A52E-89FC6130AD21}" name="Table1221" displayName="Table1221" ref="A39:C49" totalsRowShown="0" headerRowDxfId="102" headerRowBorderDxfId="101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{333F2C22-64BE-8A4A-A52E-89FC6130AD21}" name="Table1221" displayName="Table1221" ref="A39:C49" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32">
   <autoFilter ref="A39:C49" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0A95F7D5-D48D-864F-84FF-73515D627597}" name="Version" dataDxfId="100" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{0A95F7D5-D48D-864F-84FF-73515D627597}" name="Version" dataDxfId="31" dataCellStyle="Comma"/>
     <tableColumn id="2" xr3:uid="{1427474E-5614-2046-B78C-0448E419A1D9}" name="Date"/>
     <tableColumn id="3" xr3:uid="{CAF26780-3593-1540-85AB-2E9EB898659F}" name="Notes"/>
   </tableColumns>
@@ -5275,13 +4617,13 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_3" displayName="Table_3" ref="E9:K10">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Offering" dataDxfId="156"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Description" dataDxfId="155"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="154"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Dimension" dataDxfId="153"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="GB per credit" dataDxfId="152"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Quantity (GB)" dataDxfId="151"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Credits" dataDxfId="150">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Offering" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Description" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Dimension" dataDxfId="84"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="GB per credit" dataDxfId="83"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Quantity (GB)" dataDxfId="82"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Credits" dataDxfId="81">
       <calculatedColumnFormula>ROUNDUP(Table_3[[#This Row],[Quantity (GB)]]/Table_3[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5295,12 +4637,12 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Offering"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Units"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Dimension" dataDxfId="149"/>
-    <tableColumn id="3" xr3:uid="{CDA60C5E-AE6A-324F-8F61-A71F1A0A8966}" name="GB per credit" dataDxfId="148">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Dimension" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{CDA60C5E-AE6A-324F-8F61-A71F1A0A8966}" name="GB per credit" dataDxfId="79">
       <calculatedColumnFormula>'AWS Service Prices'!K5*'AWS Service Prices'!M5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Quantity (GB)" dataDxfId="147"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Credits" dataDxfId="146">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Quantity (GB)" dataDxfId="78"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Credits" dataDxfId="77">
       <calculatedColumnFormula>ROUNDUP(Table_4[[#This Row],[Quantity (GB)]]/Table_4[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5312,7 +4654,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_5" displayName="Table_5" ref="A14:C15">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Rate/Hour"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Hours" dataDxfId="145"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Hours" dataDxfId="76"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Total"/>
   </tableColumns>
   <tableStyleInfo name="Worksheet-style 5" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
@@ -5320,17 +4662,17 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_6" displayName="Table_6" ref="M14:S15" dataDxfId="144">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_6" displayName="Table_6" ref="M14:S15" dataDxfId="75">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Offering" dataDxfId="143"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Description" dataDxfId="142"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Units" dataDxfId="141"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Dimension" dataDxfId="140"/>
-    <tableColumn id="3" xr3:uid="{807927EE-801B-8148-9BA1-5FE9186170F2}" name="GB per credit" dataDxfId="139">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Offering" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Description" dataDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Units" dataDxfId="72"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Dimension" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{807927EE-801B-8148-9BA1-5FE9186170F2}" name="GB per credit" dataDxfId="70">
       <calculatedColumnFormula>'AWS Service Prices'!K4*'AWS Service Prices'!M4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Quantity (GB)" dataDxfId="138"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Credits" dataDxfId="137">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Quantity (GB)" dataDxfId="69"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Credits" dataDxfId="68">
       <calculatedColumnFormula>ROUNDUP(Table_6[[#This Row],[Quantity (GB)]]/Table_6[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5355,11 +4697,11 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Units"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Dimension"/>
-    <tableColumn id="3" xr3:uid="{A30E673E-5221-9442-BA33-5D5CC8E273B5}" name="Units/Credit" dataDxfId="136">
+    <tableColumn id="3" xr3:uid="{A30E673E-5221-9442-BA33-5D5CC8E273B5}" name="Units/Credit" dataDxfId="67">
       <calculatedColumnFormula>'AWS Service Prices'!K6*'AWS Service Prices'!M6</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Quantity"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Credits" dataDxfId="135">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Credits" dataDxfId="66">
       <calculatedColumnFormula>ROUNDUP(Table_8[[#This Row],[Quantity]]/Table_8[[#This Row],[Units/Credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5368,10 +4710,10 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}" name="Table12" displayName="Table12" ref="A40:C50" totalsRowShown="0" headerRowDxfId="134" headerRowBorderDxfId="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}" name="Table12" displayName="Table12" ref="A40:C50" totalsRowShown="0" headerRowDxfId="65" headerRowBorderDxfId="64">
   <autoFilter ref="A40:C50" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6F594386-932F-3745-B570-1D36152A4BED}" name="Version" dataDxfId="132" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{6F594386-932F-3745-B570-1D36152A4BED}" name="Version" dataDxfId="63" dataCellStyle="Comma"/>
     <tableColumn id="2" xr3:uid="{98BA1600-A7B8-2742-AF88-1C465CCF83D5}" name="Date"/>
     <tableColumn id="3" xr3:uid="{A3A06425-E98A-E042-A27B-C92165F08BCF}" name="Notes"/>
   </tableColumns>
@@ -5583,8 +4925,8 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N46" sqref="N46"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5614,14 +4956,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="98.25" customHeight="1" x14ac:dyDescent="1.05">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="125" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5656,7 +4998,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="120">
+      <c r="A5" s="118">
         <f>C10+SUM(B19:B24)</f>
         <v>0</v>
       </c>
@@ -6227,10 +5569,10 @@
       </c>
     </row>
     <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="121" t="s">
+      <c r="A22" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="122">
+      <c r="B22" s="120">
         <f>SUM(S33:S37)</f>
         <v>0</v>
       </c>
@@ -6280,10 +5622,10 @@
       </c>
     </row>
     <row r="23" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="124" t="s">
+      <c r="A23" s="122" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="123">
+      <c r="B23" s="121">
         <f>SUM(Table_8[Credits])</f>
         <v>0</v>
       </c>
@@ -6333,10 +5675,10 @@
       </c>
     </row>
     <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="126" t="s">
+      <c r="A24" s="124" t="s">
         <v>196</v>
       </c>
-      <c r="B24" s="125">
+      <c r="B24" s="123">
         <f>$P$46</f>
         <v>0</v>
       </c>
@@ -7297,11 +6639,11 @@
       <c r="P45" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="Q45" s="114" t="s">
+      <c r="Q45" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="R45" s="111"/>
-      <c r="S45" s="111"/>
+      <c r="R45" s="109"/>
+      <c r="S45" s="109"/>
     </row>
     <row r="46" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="105">
@@ -7314,24 +6656,24 @@
         <v>191</v>
       </c>
       <c r="J46" s="4"/>
-      <c r="M46" s="118" t="s">
+      <c r="M46" s="116" t="s">
         <v>196</v>
       </c>
-      <c r="N46" s="116" t="s">
+      <c r="N46" s="114" t="s">
         <v>197</v>
       </c>
-      <c r="O46" s="117">
+      <c r="O46" s="115">
         <v>1</v>
       </c>
-      <c r="P46" s="116">
-        <v>0</v>
-      </c>
-      <c r="Q46" s="119">
+      <c r="P46" s="114">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="117">
         <f>O46*P46</f>
         <v>0</v>
       </c>
-      <c r="R46" s="112"/>
-      <c r="S46" s="112"/>
+      <c r="R46" s="110"/>
+      <c r="S46" s="110"/>
     </row>
     <row r="47" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="105">
@@ -7346,11 +6688,11 @@
       <c r="J47" s="4"/>
       <c r="M47" s="88"/>
       <c r="N47" s="88"/>
-      <c r="O47" s="115"/>
+      <c r="O47" s="113"/>
       <c r="P47" s="88"/>
       <c r="Q47" s="88"/>
-      <c r="R47" s="113"/>
-      <c r="S47" s="112"/>
+      <c r="R47" s="111"/>
+      <c r="S47" s="110"/>
     </row>
     <row r="48" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="105"/>
@@ -7364,7 +6706,7 @@
         <v>1.5</v>
       </c>
       <c r="B49" s="101">
-        <v>45839</v>
+        <v>45840</v>
       </c>
       <c r="C49" s="106" t="s">
         <v>198</v>
@@ -8430,43 +7772,43 @@
       <formula>$R41&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="N46">
+    <cfRule type="expression" dxfId="21" priority="3">
+      <formula>$P$46&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P46">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="21" priority="14" operator="notEqual">
+    <cfRule type="cellIs" dxfId="19" priority="14" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R15">
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="notEqual">
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R19:R29">
-    <cfRule type="cellIs" dxfId="19" priority="16" operator="notEqual">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R33:R37">
-    <cfRule type="cellIs" dxfId="18" priority="15" operator="notEqual">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R41:R42">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N46">
-    <cfRule type="expression" dxfId="16" priority="3">
-      <formula>$P$46&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="R46:R47">
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P46">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12581,14 +11923,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="98.25" customHeight="1" x14ac:dyDescent="1.05">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="125" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Document and price domain-with-cdn-dedicated-waf plan (#145)
* update cost estimator spreadsheet to include costs for domain-with-cdn-dedicated-waf plans

* update version and updated date for cost estimator spreadsheet

* update docs on external domain service to document domain-with-cdn-dedicated-waf plan

* add documentation on alarm_notification_email parameter

* update cost estimator

* update cost estimator spreadsheet

* update page and spreadsheet to note correct date of last version update for pricing spreadsheet
</commit_message>
<xml_diff>
--- a/_assets/documents/cloud-gov-cost-estimator.xlsx
+++ b/_assets/documents/cloud-gov-cost-estimator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterdburkholder/Projects/cloud-gov/site/_assets/documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markdboyd/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5274FA16-971E-7A40-85CA-ED6AD0EAA238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C5E9B5-D04A-0047-B569-6F61061D3C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="500" windowWidth="47840" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="199">
   <si>
     <t>Estimated Price</t>
   </si>
@@ -665,6 +665,18 @@
   </si>
   <si>
     <t>Mv example to end</t>
+  </si>
+  <si>
+    <t>External domains</t>
+  </si>
+  <si>
+    <t>External domain</t>
+  </si>
+  <si>
+    <t>domain-with-cdn-dedicated-waf</t>
+  </si>
+  <si>
+    <t>Add dedicated CDN</t>
   </si>
 </sst>
 </file>
@@ -817,7 +829,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -1458,12 +1470,89 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF356854"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF284E3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF4A535C"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF6F8F9"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF6F8F9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF6F8F9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF4A535C"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF6F8F9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1744,6 +1833,53 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1753,7 +1889,304 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="122">
+  <dxfs count="125">
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <u/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="169" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -2710,272 +3143,6 @@
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="169" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -4177,54 +4344,54 @@
   </dxfs>
   <tableStyles count="10">
     <tableStyle name="Worksheet-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="124"/>
+      <tableStyleElement type="firstRowStripe" dxfId="123"/>
+      <tableStyleElement type="secondRowStripe" dxfId="122"/>
+    </tableStyle>
+    <tableStyle name="Worksheet-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="headerRow" dxfId="121"/>
       <tableStyleElement type="firstRowStripe" dxfId="120"/>
       <tableStyleElement type="secondRowStripe" dxfId="119"/>
     </tableStyle>
-    <tableStyle name="Worksheet-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+    <tableStyle name="Worksheet-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
       <tableStyleElement type="headerRow" dxfId="118"/>
       <tableStyleElement type="firstRowStripe" dxfId="117"/>
       <tableStyleElement type="secondRowStripe" dxfId="116"/>
     </tableStyle>
-    <tableStyle name="Worksheet-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
+    <tableStyle name="Worksheet-style 4" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
       <tableStyleElement type="headerRow" dxfId="115"/>
       <tableStyleElement type="firstRowStripe" dxfId="114"/>
       <tableStyleElement type="secondRowStripe" dxfId="113"/>
     </tableStyle>
-    <tableStyle name="Worksheet-style 4" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
+    <tableStyle name="Worksheet-style 5" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
       <tableStyleElement type="headerRow" dxfId="112"/>
       <tableStyleElement type="firstRowStripe" dxfId="111"/>
       <tableStyleElement type="secondRowStripe" dxfId="110"/>
     </tableStyle>
-    <tableStyle name="Worksheet-style 5" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
+    <tableStyle name="Worksheet-style 6" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
       <tableStyleElement type="headerRow" dxfId="109"/>
       <tableStyleElement type="firstRowStripe" dxfId="108"/>
       <tableStyleElement type="secondRowStripe" dxfId="107"/>
     </tableStyle>
-    <tableStyle name="Worksheet-style 6" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
+    <tableStyle name="Worksheet-style 7" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF06000000}">
       <tableStyleElement type="headerRow" dxfId="106"/>
       <tableStyleElement type="firstRowStripe" dxfId="105"/>
       <tableStyleElement type="secondRowStripe" dxfId="104"/>
     </tableStyle>
-    <tableStyle name="Worksheet-style 7" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF06000000}">
+    <tableStyle name="Worksheet-style 8" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF07000000}">
       <tableStyleElement type="headerRow" dxfId="103"/>
       <tableStyleElement type="firstRowStripe" dxfId="102"/>
       <tableStyleElement type="secondRowStripe" dxfId="101"/>
     </tableStyle>
-    <tableStyle name="Worksheet-style 8" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF07000000}">
+    <tableStyle name="Cloud.gov Tiers-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF08000000}">
       <tableStyleElement type="headerRow" dxfId="100"/>
       <tableStyleElement type="firstRowStripe" dxfId="99"/>
       <tableStyleElement type="secondRowStripe" dxfId="98"/>
     </tableStyle>
-    <tableStyle name="Cloud.gov Tiers-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF08000000}">
+    <tableStyle name="Cloud.gov Tiers-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF09000000}">
       <tableStyleElement type="headerRow" dxfId="97"/>
       <tableStyleElement type="firstRowStripe" dxfId="96"/>
       <tableStyleElement type="secondRowStripe" dxfId="95"/>
-    </tableStyle>
-    <tableStyle name="Cloud.gov Tiers-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF09000000}">
-      <tableStyleElement type="headerRow" dxfId="94"/>
-      <tableStyleElement type="firstRowStripe" dxfId="93"/>
-      <tableStyleElement type="secondRowStripe" dxfId="92"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -4241,20 +4408,20 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A4:F5">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Credits" dataDxfId="91"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tier Name" dataDxfId="90">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Credits" dataDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tier Name" dataDxfId="93">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.Tier, VLOOKUP(MIN(IF('Cloud.gov Tiers'!$B$11:$B$28&gt;=A5, 'Cloud.gov Tiers'!$B$11:$B$28)), 'Cloud.gov Tiers'!$B$11:$E$28, 4, FALSE), VLOOKUP(_xlpm.Tier, 'Cloud.gov Tiers'!$E$10:$F$28, 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Credits Remaining_x000a_in Tier" dataDxfId="89">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Credits Remaining_x000a_in Tier" dataDxfId="92">
       <calculatedColumnFormula>VLOOKUP(Table_1[[#This Row],[Tier Name]], 'Cloud.gov Tiers'!A11:B27, 2,FALSE)-Table_1[[#This Row],[Credits]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Yearly_x000a_Platform Total" dataDxfId="88">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Yearly_x000a_Platform Total" dataDxfId="91">
       <calculatedColumnFormula>IF(B5="Custom", ROUNDUP(A5/1000,0)*'Cloud.gov Tiers'!$H$28, VLOOKUP(B5, 'Cloud.gov Tiers'!$F$11:$H$27, 3, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Support Total" dataDxfId="87">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Support Total" dataDxfId="90">
       <calculatedColumnFormula>C15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name=" YearlyTotal Cost" dataDxfId="86">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name=" YearlyTotal Cost" dataDxfId="89">
       <calculatedColumnFormula>D5+E5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4291,22 +4458,22 @@
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{4C37D040-F691-2C49-BE22-816489BFD4D2}" name="Table_112" displayName="Table_112" ref="A4:F5">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{657244D4-FE4C-D44C-B48B-43E7FA139C6B}" name="Credits" dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{657244D4-FE4C-D44C-B48B-43E7FA139C6B}" name="Credits" dataDxfId="62">
       <calculatedColumnFormula>C10+SUM(B19:B23)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B168D809-F848-8A4F-B241-57C6EF027C29}" name="Tier Name" dataDxfId="30">
+    <tableColumn id="2" xr3:uid="{B168D809-F848-8A4F-B241-57C6EF027C29}" name="Tier Name" dataDxfId="61">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.Tier, VLOOKUP(MIN(IF('Cloud.gov Tiers'!$B$11:$B$28&gt;=A5, 'Cloud.gov Tiers'!$B$11:$B$28)), 'Cloud.gov Tiers'!$B$11:$E$28, 4, FALSE), VLOOKUP(_xlpm.Tier, 'Cloud.gov Tiers'!$E$10:$F$28, 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{172BAC85-F7D2-7D4C-9C26-72C7C85DB56F}" name="Credits Remaining_x000a_in Tier" dataDxfId="29">
+    <tableColumn id="3" xr3:uid="{172BAC85-F7D2-7D4C-9C26-72C7C85DB56F}" name="Credits Remaining_x000a_in Tier" dataDxfId="60">
       <calculatedColumnFormula>VLOOKUP(Table_112[[#This Row],[Tier Name]], 'Cloud.gov Tiers'!A11:B27, 2,FALSE)-Table_112[[#This Row],[Credits]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{19498A2C-21A7-B740-9DD5-D095ED0DD812}" name="Yearly_x000a_Platform Total" dataDxfId="28">
+    <tableColumn id="4" xr3:uid="{19498A2C-21A7-B740-9DD5-D095ED0DD812}" name="Yearly_x000a_Platform Total" dataDxfId="59">
       <calculatedColumnFormula>IF(B5="Custom", ROUNDUP(A5/1000,0)*'Cloud.gov Tiers'!$H$28, VLOOKUP(B5, 'Cloud.gov Tiers'!$F$11:$H$27, 3, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{A475BA76-45A9-EF46-8FAE-2B381389CF6E}" name="Support Total" dataDxfId="27">
+    <tableColumn id="5" xr3:uid="{A475BA76-45A9-EF46-8FAE-2B381389CF6E}" name="Support Total" dataDxfId="58">
       <calculatedColumnFormula>C15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{CFD58EB9-7FC4-3640-859D-34D006952E97}" name=" YearlyTotal Cost" dataDxfId="26">
+    <tableColumn id="6" xr3:uid="{CFD58EB9-7FC4-3640-859D-34D006952E97}" name=" YearlyTotal Cost" dataDxfId="57">
       <calculatedColumnFormula>D5+E5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4318,7 +4485,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{432B26DD-C481-9945-89E7-FEF42FEDB769}" name="Table_214" displayName="Table_214" ref="A9:C10">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8D2D857E-9AA6-5D4F-A4AF-373B7168526E}" name="Resource"/>
-    <tableColumn id="2" xr3:uid="{4FAE5D4B-8591-7D41-A69E-501EE57C6C41}" name="Quantity" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{4FAE5D4B-8591-7D41-A69E-501EE57C6C41}" name="Quantity" dataDxfId="56"/>
     <tableColumn id="3" xr3:uid="{FD66B2C4-D49F-1C43-9A30-DE1F21B9FD5B}" name="Credits">
       <calculatedColumnFormula>B10*'Cloud.gov Tiers'!B3</calculatedColumnFormula>
     </tableColumn>
@@ -4330,13 +4497,13 @@
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{3AE58A18-ABB7-FC4E-9D28-06F1CAA78773}" name="Table_315" displayName="Table_315" ref="E9:K10">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8901DDBE-58BA-8F4F-9D7C-2A2800A70157}" name="Offering" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{3C07AF3B-6C04-4348-A1E4-AEF634AB5F2C}" name="Description" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{50B2B6E3-7A84-CC41-A61F-9E7C70E4AC01}" name="Units" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{99748816-FA07-B948-9F02-BAFA13C63BF0}" name="Dimension" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{B4686AED-FFA8-0F4F-8CF1-A28CBB869F59}" name="GB per credit" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{C47C64B0-2C30-0043-A34C-7F0E810B25DC}" name="Quantity (GB)" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{D0A5DC61-9EB0-294B-94B0-91D19A5D6E7E}" name="Credits" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{8901DDBE-58BA-8F4F-9D7C-2A2800A70157}" name="Offering" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{3C07AF3B-6C04-4348-A1E4-AEF634AB5F2C}" name="Description" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{50B2B6E3-7A84-CC41-A61F-9E7C70E4AC01}" name="Units" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{99748816-FA07-B948-9F02-BAFA13C63BF0}" name="Dimension" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{B4686AED-FFA8-0F4F-8CF1-A28CBB869F59}" name="GB per credit" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{C47C64B0-2C30-0043-A34C-7F0E810B25DC}" name="Quantity (GB)" dataDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{D0A5DC61-9EB0-294B-94B0-91D19A5D6E7E}" name="Credits" dataDxfId="49">
       <calculatedColumnFormula>ROUNDUP(Table_315[[#This Row],[Quantity (GB)]]/Table_315[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4350,12 +4517,12 @@
     <tableColumn id="1" xr3:uid="{CC812881-5649-1A4C-8C45-49D7808E0D1A}" name="Offering"/>
     <tableColumn id="2" xr3:uid="{46204D59-C3E2-174B-9C58-1DB2BB6988C8}" name="Description"/>
     <tableColumn id="4" xr3:uid="{C3D129A0-D876-D446-9BED-4CE757DA989E}" name="Units"/>
-    <tableColumn id="5" xr3:uid="{8159B7E1-3CBB-384F-9C82-294839F55CB1}" name="Dimension" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{6374D1D7-2C6C-674A-9B2C-B5EA274BAEAC}" name="GB per credit" dataDxfId="16">
+    <tableColumn id="5" xr3:uid="{8159B7E1-3CBB-384F-9C82-294839F55CB1}" name="Dimension" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{6374D1D7-2C6C-674A-9B2C-B5EA274BAEAC}" name="GB per credit" dataDxfId="47">
       <calculatedColumnFormula>'AWS Service Prices'!K5*'AWS Service Prices'!M5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{84537EB8-58A4-A645-9A18-A322EFB5D6C3}" name="Quantity (GB)" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{06CE2B03-0479-2148-9683-4F1675E4317C}" name="Credits" dataDxfId="14">
+    <tableColumn id="6" xr3:uid="{84537EB8-58A4-A645-9A18-A322EFB5D6C3}" name="Quantity (GB)" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{06CE2B03-0479-2148-9683-4F1675E4317C}" name="Credits" dataDxfId="45">
       <calculatedColumnFormula>ROUNDUP(Table_416[[#This Row],[Quantity (GB)]]/Table_416[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4367,7 +4534,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{DD38669A-9AE2-BA49-AF4A-F9D5CEFDB233}" name="Table_517" displayName="Table_517" ref="A14:C15">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E0798FE9-1580-1B43-B088-25897B8976F6}" name="Rate/Hour"/>
-    <tableColumn id="2" xr3:uid="{4F69F05E-31AF-C644-B087-9847D08BB3A0}" name="Hours" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{4F69F05E-31AF-C644-B087-9847D08BB3A0}" name="Hours" dataDxfId="44"/>
     <tableColumn id="3" xr3:uid="{35F99F2C-96B5-1244-8BF2-D8FA71D1A5B2}" name="Total">
       <calculatedColumnFormula>A15*B15</calculatedColumnFormula>
     </tableColumn>
@@ -4377,17 +4544,17 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{53A578BF-BA5A-7843-972B-EBD4EA7AD1DD}" name="Table_618" displayName="Table_618" ref="M14:S15" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{53A578BF-BA5A-7843-972B-EBD4EA7AD1DD}" name="Table_618" displayName="Table_618" ref="M14:S15" dataDxfId="43">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3024083C-5ED0-8D4D-8D1A-D4BD5916AE47}" name="Offering" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{3D92B04D-745E-2A49-991D-C00C27907719}" name="Description" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{50C39022-EBD5-9B42-84DD-C507ED702117}" name="Units" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{9759566D-ABA1-0943-92F2-2B5501002EE3}" name="Dimension" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{4A17BDB6-3CD8-BF43-B5F9-82D2A2C35A0C}" name="GB per credit" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{3024083C-5ED0-8D4D-8D1A-D4BD5916AE47}" name="Offering" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{3D92B04D-745E-2A49-991D-C00C27907719}" name="Description" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{50C39022-EBD5-9B42-84DD-C507ED702117}" name="Units" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{9759566D-ABA1-0943-92F2-2B5501002EE3}" name="Dimension" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{4A17BDB6-3CD8-BF43-B5F9-82D2A2C35A0C}" name="GB per credit" dataDxfId="38">
       <calculatedColumnFormula>'AWS Service Prices'!K4*'AWS Service Prices'!M4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{056FCEF1-5646-814F-8034-1E8AC53C910D}" name="Quantity (GB)" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{DAEA814F-05EA-764E-8533-FE0EF6F3B132}" name="Credits" dataDxfId="5">
+    <tableColumn id="6" xr3:uid="{056FCEF1-5646-814F-8034-1E8AC53C910D}" name="Quantity (GB)" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{DAEA814F-05EA-764E-8533-FE0EF6F3B132}" name="Credits" dataDxfId="36">
       <calculatedColumnFormula>ROUNDUP(Table_618[[#This Row],[Quantity (GB)]]/Table_618[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4412,11 +4579,11 @@
     <tableColumn id="2" xr3:uid="{B074D0B3-B914-AB4F-8066-81B90B3261D8}" name="Description"/>
     <tableColumn id="4" xr3:uid="{202C8C30-FD4E-6D40-9EBF-642B8C7AE181}" name="Units"/>
     <tableColumn id="5" xr3:uid="{CA6A3A17-2747-AF44-8119-FC05700B8D5C}" name="Dimension"/>
-    <tableColumn id="3" xr3:uid="{C6C6ED4B-9612-3F48-9D18-472E70646A28}" name="Units/Credit" dataDxfId="4">
+    <tableColumn id="3" xr3:uid="{C6C6ED4B-9612-3F48-9D18-472E70646A28}" name="Units/Credit" dataDxfId="35">
       <calculatedColumnFormula>'AWS Service Prices'!K6*'AWS Service Prices'!M6</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{76CCCB3A-2B18-4C42-9DB6-C570AFD6FB75}" name="Quantity"/>
-    <tableColumn id="7" xr3:uid="{A024F374-2C63-444D-95DA-745B84ABCFE7}" name="Credits" dataDxfId="3">
+    <tableColumn id="7" xr3:uid="{A024F374-2C63-444D-95DA-745B84ABCFE7}" name="Credits" dataDxfId="34">
       <calculatedColumnFormula>ROUNDUP(Table_820[[#This Row],[Quantity]]/Table_820[[#This Row],[Units/Credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4428,7 +4595,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A9:C10">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Resource"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Quantity" dataDxfId="85"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Quantity" dataDxfId="88"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Credits"/>
   </tableColumns>
   <tableStyleInfo name="Worksheet-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
@@ -4436,10 +4603,10 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{333F2C22-64BE-8A4A-A52E-89FC6130AD21}" name="Table1221" displayName="Table1221" ref="A39:C49" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{333F2C22-64BE-8A4A-A52E-89FC6130AD21}" name="Table1221" displayName="Table1221" ref="A39:C49" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32">
   <autoFilter ref="A39:C49" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0A95F7D5-D48D-864F-84FF-73515D627597}" name="Version" dataDxfId="0" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{0A95F7D5-D48D-864F-84FF-73515D627597}" name="Version" dataDxfId="31" dataCellStyle="Comma"/>
     <tableColumn id="2" xr3:uid="{1427474E-5614-2046-B78C-0448E419A1D9}" name="Date"/>
     <tableColumn id="3" xr3:uid="{CAF26780-3593-1540-85AB-2E9EB898659F}" name="Notes"/>
   </tableColumns>
@@ -4450,13 +4617,13 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_3" displayName="Table_3" ref="E9:K10">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Offering" dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Description" dataDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="82"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Dimension" dataDxfId="81"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="GB per credit" dataDxfId="80"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Quantity (GB)" dataDxfId="79"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Credits" dataDxfId="78">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Offering" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Description" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Dimension" dataDxfId="84"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="GB per credit" dataDxfId="83"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Quantity (GB)" dataDxfId="82"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Credits" dataDxfId="81">
       <calculatedColumnFormula>ROUNDUP(Table_3[[#This Row],[Quantity (GB)]]/Table_3[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4470,12 +4637,12 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Offering"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Units"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Dimension" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{CDA60C5E-AE6A-324F-8F61-A71F1A0A8966}" name="GB per credit" dataDxfId="76">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Dimension" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{CDA60C5E-AE6A-324F-8F61-A71F1A0A8966}" name="GB per credit" dataDxfId="79">
       <calculatedColumnFormula>'AWS Service Prices'!K5*'AWS Service Prices'!M5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Quantity (GB)" dataDxfId="75"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Credits" dataDxfId="74">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Quantity (GB)" dataDxfId="78"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Credits" dataDxfId="77">
       <calculatedColumnFormula>ROUNDUP(Table_4[[#This Row],[Quantity (GB)]]/Table_4[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4487,7 +4654,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_5" displayName="Table_5" ref="A14:C15">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Rate/Hour"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Hours" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Hours" dataDxfId="76"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Total"/>
   </tableColumns>
   <tableStyleInfo name="Worksheet-style 5" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
@@ -4495,17 +4662,17 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_6" displayName="Table_6" ref="M14:S15" dataDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_6" displayName="Table_6" ref="M14:S15" dataDxfId="75">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Offering" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Description" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Units" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Dimension" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{807927EE-801B-8148-9BA1-5FE9186170F2}" name="GB per credit" dataDxfId="67">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Offering" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Description" dataDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Units" dataDxfId="72"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Dimension" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{807927EE-801B-8148-9BA1-5FE9186170F2}" name="GB per credit" dataDxfId="70">
       <calculatedColumnFormula>'AWS Service Prices'!K4*'AWS Service Prices'!M4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Quantity (GB)" dataDxfId="66"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Credits" dataDxfId="65">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Quantity (GB)" dataDxfId="69"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Credits" dataDxfId="68">
       <calculatedColumnFormula>ROUNDUP(Table_6[[#This Row],[Quantity (GB)]]/Table_6[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4514,7 +4681,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table_7" displayName="Table_7" ref="A18:B23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table_7" displayName="Table_7" ref="A18:B24">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Service"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Credits"/>
@@ -4530,11 +4697,11 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Units"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Dimension"/>
-    <tableColumn id="3" xr3:uid="{A30E673E-5221-9442-BA33-5D5CC8E273B5}" name="Units/Credit" dataDxfId="64">
+    <tableColumn id="3" xr3:uid="{A30E673E-5221-9442-BA33-5D5CC8E273B5}" name="Units/Credit" dataDxfId="67">
       <calculatedColumnFormula>'AWS Service Prices'!K6*'AWS Service Prices'!M6</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Quantity"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Credits" dataDxfId="63">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Credits" dataDxfId="66">
       <calculatedColumnFormula>ROUNDUP(Table_8[[#This Row],[Quantity]]/Table_8[[#This Row],[Units/Credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4543,10 +4710,10 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}" name="Table12" displayName="Table12" ref="A39:C49" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61">
-  <autoFilter ref="A39:C49" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}" name="Table12" displayName="Table12" ref="A40:C50" totalsRowShown="0" headerRowDxfId="65" headerRowBorderDxfId="64">
+  <autoFilter ref="A40:C50" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6F594386-932F-3745-B570-1D36152A4BED}" name="Version" dataDxfId="60" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{6F594386-932F-3745-B570-1D36152A4BED}" name="Version" dataDxfId="63" dataCellStyle="Comma"/>
     <tableColumn id="2" xr3:uid="{98BA1600-A7B8-2742-AF88-1C465CCF83D5}" name="Date"/>
     <tableColumn id="3" xr3:uid="{A3A06425-E98A-E042-A27B-C92165F08BCF}" name="Notes"/>
   </tableColumns>
@@ -4758,8 +4925,8 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4789,14 +4956,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="98.25" customHeight="1" x14ac:dyDescent="1.05">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="125" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4831,8 +4998,8 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="81">
-        <f>C10+SUM(B19:B23)</f>
+      <c r="A5" s="118">
+        <f>C10+SUM(B19:B24)</f>
         <v>0</v>
       </c>
       <c r="B5" s="82" t="str" cm="1">
@@ -5402,10 +5569,10 @@
       </c>
     </row>
     <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="34">
+      <c r="B22" s="120">
         <f>SUM(S33:S37)</f>
         <v>0</v>
       </c>
@@ -5455,10 +5622,10 @@
       </c>
     </row>
     <row r="23" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="122" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="37">
+      <c r="B23" s="121">
         <f>SUM(Table_8[Credits])</f>
         <v>0</v>
       </c>
@@ -5508,6 +5675,13 @@
       </c>
     </row>
     <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="124" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" s="123">
+        <f>$P$46</f>
+        <v>0</v>
+      </c>
       <c r="E24" s="18" t="str">
         <v>AWS RDS</v>
       </c>
@@ -5600,9 +5774,6 @@
       </c>
     </row>
     <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="28" t="s">
-        <v>174</v>
-      </c>
       <c r="E26" s="18" t="str">
         <v>AWS RDS</v>
       </c>
@@ -5650,10 +5821,7 @@
     </row>
     <row r="27" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="28" t="s">
-        <v>23</v>
+        <v>174</v>
       </c>
       <c r="E27" s="24" t="str">
         <v>AWS RDS</v>
@@ -5701,12 +5869,11 @@
       </c>
     </row>
     <row r="28" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="18" t="str">
-        <f t="array" ref="A28:B35">CloudGovNoCostServices</f>
-        <v>External Domain</v>
-      </c>
-      <c r="B28" s="21" t="str">
-        <v>cdn-route</v>
+      <c r="A28" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>23</v>
       </c>
       <c r="E28" s="18" t="str">
         <v>AWS RDS</v>
@@ -5754,11 +5921,12 @@
       </c>
     </row>
     <row r="29" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="24" t="str">
+      <c r="A29" s="18" t="str">
+        <f t="array" ref="A29:B36">CloudGovNoCostServices</f>
         <v>External Domain</v>
       </c>
-      <c r="B29" s="27" t="str">
-        <v>custom-domain</v>
+      <c r="B29" s="21" t="str">
+        <v>cdn-route</v>
       </c>
       <c r="E29" s="24" t="str">
         <v>AWS RDS</v>
@@ -5807,11 +5975,11 @@
       <c r="T29" s="92"/>
     </row>
     <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="18" t="str">
+      <c r="A30" s="24" t="str">
         <v>External Domain</v>
       </c>
-      <c r="B30" s="21" t="str">
-        <v>domain</v>
+      <c r="B30" s="27" t="str">
+        <v>custom-domain</v>
       </c>
       <c r="E30" s="18" t="str">
         <v>AWS RDS</v>
@@ -5839,11 +6007,11 @@
       <c r="Y30" s="29"/>
     </row>
     <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="24" t="str">
+      <c r="A31" s="18" t="str">
         <v>External Domain</v>
       </c>
-      <c r="B31" s="27" t="str">
-        <v>domain-with-cdn</v>
+      <c r="B31" s="21" t="str">
+        <v>domain</v>
       </c>
       <c r="E31" s="24" t="str">
         <v>AWS RDS</v>
@@ -5877,11 +6045,11 @@
       <c r="R31" s="87"/>
     </row>
     <row r="32" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="18" t="str">
-        <v>UAA Service Account</v>
-      </c>
-      <c r="B32" s="21" t="str">
-        <v>oauth-client</v>
+      <c r="A32" s="24" t="str">
+        <v>External Domain</v>
+      </c>
+      <c r="B32" s="27" t="str">
+        <v>domain-with-cdn</v>
       </c>
       <c r="E32" s="18" t="str">
         <v>AWS RDS</v>
@@ -5928,11 +6096,11 @@
       </c>
     </row>
     <row r="33" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="24" t="str">
+      <c r="A33" s="18" t="str">
         <v>UAA Service Account</v>
       </c>
-      <c r="B33" s="27" t="str">
-        <v>space-auditor</v>
+      <c r="B33" s="21" t="str">
+        <v>oauth-client</v>
       </c>
       <c r="E33" s="24" t="str">
         <v>AWS RDS</v>
@@ -5981,11 +6149,11 @@
       </c>
     </row>
     <row r="34" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="18" t="str">
+      <c r="A34" s="24" t="str">
         <v>UAA Service Account</v>
       </c>
-      <c r="B34" s="21" t="str">
-        <v>space-deployer</v>
+      <c r="B34" s="27" t="str">
+        <v>space-auditor</v>
       </c>
       <c r="E34" s="18" t="str">
         <v>AWS RDS</v>
@@ -6033,11 +6201,11 @@
       </c>
     </row>
     <row r="35" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="24" t="str">
-        <v>Autoscaler</v>
-      </c>
-      <c r="B35" s="27" t="str">
-        <v>autoscaler-free-plan</v>
+      <c r="A35" s="18" t="str">
+        <v>UAA Service Account</v>
+      </c>
+      <c r="B35" s="21" t="str">
+        <v>space-deployer</v>
       </c>
       <c r="E35" s="24" t="str">
         <v>AWS RDS</v>
@@ -6085,10 +6253,12 @@
       </c>
     </row>
     <row r="36" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="B36" s="44"/>
+      <c r="A36" s="24" t="str">
+        <v>Autoscaler</v>
+      </c>
+      <c r="B36" s="27" t="str">
+        <v>autoscaler-free-plan</v>
+      </c>
       <c r="E36" s="18" t="str">
         <v>AWS RDS</v>
       </c>
@@ -6135,6 +6305,10 @@
       </c>
     </row>
     <row r="37" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" s="44"/>
       <c r="E37" s="24" t="str">
         <v>AWS RDS</v>
       </c>
@@ -6205,15 +6379,6 @@
       </c>
     </row>
     <row r="39" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="102" t="s">
-        <v>183</v>
-      </c>
-      <c r="B39" s="103" t="s">
-        <v>184</v>
-      </c>
-      <c r="C39" s="104" t="s">
-        <v>185</v>
-      </c>
       <c r="E39" s="24" t="str">
         <v>AWS RDS</v>
       </c>
@@ -6241,14 +6406,14 @@
       </c>
     </row>
     <row r="40" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="105">
-        <v>1</v>
-      </c>
-      <c r="B40" s="101">
-        <v>45748</v>
-      </c>
-      <c r="C40" s="100" t="s">
-        <v>189</v>
+      <c r="A40" s="102" t="s">
+        <v>183</v>
+      </c>
+      <c r="B40" s="103" t="s">
+        <v>184</v>
+      </c>
+      <c r="C40" s="104" t="s">
+        <v>185</v>
       </c>
       <c r="E40" s="18" t="str">
         <v>AWS RDS</v>
@@ -6296,13 +6461,13 @@
     </row>
     <row r="41" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A41" s="105">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="B41" s="101">
-        <v>45749</v>
+        <v>45748</v>
       </c>
       <c r="C41" s="100" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E41" s="24" t="str">
         <v>AWS RDS</v>
@@ -6351,9 +6516,14 @@
       </c>
     </row>
     <row r="42" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="105"/>
+      <c r="A42" s="105">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B42" s="101">
+        <v>45749</v>
+      </c>
       <c r="C42" s="100" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E42" s="18" t="str">
         <v>AWS RDS</v>
@@ -6404,7 +6574,7 @@
     <row r="43" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A43" s="105"/>
       <c r="C43" s="100" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E43" s="54" t="str">
         <v>AWS RDS</v>
@@ -6431,54 +6601,116 @@
       <c r="Q43" s="98"/>
     </row>
     <row r="44" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="105">
-        <v>1.2</v>
-      </c>
-      <c r="B44" s="101">
-        <v>45756</v>
-      </c>
-      <c r="C44" s="106" t="s">
-        <v>190</v>
+      <c r="A44" s="105"/>
+      <c r="C44" s="100" t="s">
+        <v>188</v>
       </c>
       <c r="J44" s="4"/>
+      <c r="M44" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="N44" s="108"/>
+      <c r="O44" s="108"/>
+      <c r="P44" s="108"/>
+      <c r="Q44" s="108"/>
+      <c r="R44" s="108"/>
+      <c r="S44" s="108"/>
     </row>
     <row r="45" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="105">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="B45" s="101">
-        <v>45757</v>
+        <v>45756</v>
       </c>
       <c r="C45" s="106" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J45" s="4"/>
+      <c r="M45" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="N45" s="95" t="s">
+        <v>23</v>
+      </c>
+      <c r="O45" s="95" t="s">
+        <v>179</v>
+      </c>
+      <c r="P45" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q45" s="112" t="s">
+        <v>1</v>
+      </c>
+      <c r="R45" s="109"/>
+      <c r="S45" s="109"/>
     </row>
     <row r="46" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="105">
+        <v>1.3</v>
+      </c>
+      <c r="B46" s="101">
+        <v>45757</v>
+      </c>
+      <c r="C46" s="106" t="s">
+        <v>191</v>
+      </c>
+      <c r="J46" s="4"/>
+      <c r="M46" s="116" t="s">
+        <v>196</v>
+      </c>
+      <c r="N46" s="114" t="s">
+        <v>197</v>
+      </c>
+      <c r="O46" s="115">
+        <v>1</v>
+      </c>
+      <c r="P46" s="114">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="117">
+        <f>O46*P46</f>
+        <v>0</v>
+      </c>
+      <c r="R46" s="110"/>
+      <c r="S46" s="110"/>
+    </row>
+    <row r="47" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="105">
         <v>1.4</v>
       </c>
-      <c r="B46" s="101">
+      <c r="B47" s="101">
         <v>45775</v>
       </c>
-      <c r="C46" s="106" t="s">
+      <c r="C47" s="106" t="s">
         <v>193</v>
       </c>
-      <c r="J46" s="4"/>
-    </row>
-    <row r="47" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="105"/>
-      <c r="C47" s="106" t="s">
-        <v>194</v>
-      </c>
       <c r="J47" s="4"/>
+      <c r="M47" s="88"/>
+      <c r="N47" s="88"/>
+      <c r="O47" s="113"/>
+      <c r="P47" s="88"/>
+      <c r="Q47" s="88"/>
+      <c r="R47" s="111"/>
+      <c r="S47" s="110"/>
     </row>
     <row r="48" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="105"/>
+      <c r="C48" s="106" t="s">
+        <v>194</v>
+      </c>
       <c r="J48" s="4"/>
     </row>
     <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="105"/>
+      <c r="A49" s="105">
+        <v>1.5</v>
+      </c>
+      <c r="B49" s="101">
+        <v>45840</v>
+      </c>
+      <c r="C49" s="106" t="s">
+        <v>198</v>
+      </c>
       <c r="J49" s="4"/>
     </row>
     <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7496,72 +7728,87 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="B10 J14:J43 B15">
-    <cfRule type="cellIs" dxfId="59" priority="17" operator="notEqual">
+    <cfRule type="cellIs" dxfId="30" priority="21" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="58" priority="6">
+    <cfRule type="expression" dxfId="29" priority="10">
       <formula>$J$10&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:F43">
-    <cfRule type="expression" dxfId="57" priority="7">
+    <cfRule type="expression" dxfId="28" priority="11">
       <formula>$J14&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="56" priority="8" operator="notEqual">
+    <cfRule type="cellIs" dxfId="27" priority="12" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="expression" dxfId="55" priority="4">
+    <cfRule type="expression" dxfId="26" priority="8">
       <formula>$R10&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15">
-    <cfRule type="expression" dxfId="54" priority="5">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>$R15&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19:N29">
-    <cfRule type="expression" dxfId="53" priority="3">
+    <cfRule type="expression" dxfId="24" priority="7">
       <formula>$R19&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N33:N37">
-    <cfRule type="expression" dxfId="52" priority="2">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>$R33&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N41:N42">
-    <cfRule type="expression" dxfId="51" priority="1">
+    <cfRule type="expression" dxfId="22" priority="5">
       <formula>$R41&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="N46">
+    <cfRule type="expression" dxfId="21" priority="3">
+      <formula>$P$46&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P46">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="50" priority="10" operator="notEqual">
+    <cfRule type="cellIs" dxfId="19" priority="14" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R15">
-    <cfRule type="cellIs" dxfId="49" priority="9" operator="notEqual">
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R19:R29">
-    <cfRule type="cellIs" dxfId="48" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R33:R37">
-    <cfRule type="cellIs" dxfId="47" priority="11" operator="notEqual">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R41:R42">
-    <cfRule type="cellIs" dxfId="46" priority="14" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R46:R47">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11676,14 +11923,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="98.25" customHeight="1" x14ac:dyDescent="1.05">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="125" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14365,72 +14612,72 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="B10 J14:J43 B15">
-    <cfRule type="cellIs" dxfId="45" priority="14" operator="notEqual">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="44" priority="6">
+    <cfRule type="expression" dxfId="12" priority="6">
       <formula>$J$10&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:F43">
-    <cfRule type="expression" dxfId="43" priority="7">
+    <cfRule type="expression" dxfId="11" priority="7">
       <formula>$J14&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="42" priority="8" operator="notEqual">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="expression" dxfId="41" priority="4">
+    <cfRule type="expression" dxfId="9" priority="4">
       <formula>$R10&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15">
-    <cfRule type="expression" dxfId="40" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>$R15&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19:N29">
-    <cfRule type="expression" dxfId="39" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$R19&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N33:N37">
-    <cfRule type="expression" dxfId="38" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$R33&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N41:N42">
-    <cfRule type="expression" dxfId="37" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$R41&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="36" priority="10" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R15">
-    <cfRule type="cellIs" dxfId="35" priority="9" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R19:R29">
-    <cfRule type="cellIs" dxfId="34" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="12" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R33:R37">
-    <cfRule type="cellIs" dxfId="33" priority="11" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R41:R42">
-    <cfRule type="cellIs" dxfId="32" priority="13" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="13" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>